<commit_message>
Cutting out the last couple of lines
</commit_message>
<xml_diff>
--- a/data/watercorp_tanks_qpcr_raw_data.xlsx
+++ b/data/watercorp_tanks_qpcr_raw_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/NAT CSIRO/GSTWS_Tanks_Manuscript/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natnatraspberry/Desktop/Working Folder/week4_own_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334BC21C-B015-F741-9BEC-E70169365465}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A48626-EB90-744E-A3F1-607698EE613D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tanks 2017" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="144">
   <si>
     <t>Label on Tubes</t>
   </si>
@@ -963,12 +963,42 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -979,36 +1009,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1295,8 +1295,8 @@
   </sheetPr>
   <dimension ref="A1:X59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q50" sqref="Q50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1373,7 +1373,7 @@
       <c r="P1" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="Q1" s="16" t="s">
+      <c r="Q1" s="67" t="s">
         <v>78</v>
       </c>
       <c r="R1" s="14" t="s">
@@ -1394,7 +1394,7 @@
       <c r="W1" s="67" t="s">
         <v>75</v>
       </c>
-      <c r="X1" s="16" t="s">
+      <c r="X1" s="67" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1405,23 +1405,23 @@
       <c r="B2" s="1">
         <v>42947</v>
       </c>
-      <c r="C2" s="81">
+      <c r="C2" s="68">
         <v>12</v>
       </c>
-      <c r="D2" s="81">
+      <c r="D2" s="68">
         <v>56</v>
       </c>
-      <c r="E2" s="81">
+      <c r="E2" s="68">
         <v>0.56999999999999995</v>
       </c>
-      <c r="F2" s="81">
+      <c r="F2" s="68">
         <v>0.69</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="71" t="s">
+      <c r="I2" s="81" t="s">
         <v>71</v>
       </c>
       <c r="J2" s="30" t="s">
@@ -1449,18 +1449,21 @@
       <c r="W2" s="61" t="s">
         <v>141</v>
       </c>
+      <c r="X2" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="3" spans="1:24">
       <c r="A3" s="5"/>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="82"/>
-      <c r="F3" s="82"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="72"/>
+      <c r="I3" s="82"/>
       <c r="J3" s="30" t="s">
         <v>80</v>
       </c>
@@ -1486,18 +1489,21 @@
       <c r="W3" s="61" t="s">
         <v>141</v>
       </c>
+      <c r="X3" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="4" spans="1:24">
       <c r="A4" s="5"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="82"/>
-      <c r="E4" s="82"/>
-      <c r="F4" s="82"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="72"/>
+      <c r="I4" s="82"/>
       <c r="J4" s="30" t="s">
         <v>80</v>
       </c>
@@ -1523,18 +1529,21 @@
       <c r="W4" s="4" t="s">
         <v>80</v>
       </c>
+      <c r="X4" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="5" spans="1:24">
       <c r="A5" s="5"/>
-      <c r="C5" s="82"/>
-      <c r="D5" s="82"/>
-      <c r="E5" s="82"/>
-      <c r="F5" s="82"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="72"/>
+      <c r="I5" s="82"/>
       <c r="J5" s="30" t="s">
         <v>80</v>
       </c>
@@ -1560,19 +1569,22 @@
       <c r="W5" s="61" t="s">
         <v>141</v>
       </c>
+      <c r="X5" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="6" spans="1:24" s="2" customFormat="1" ht="16" thickBot="1">
       <c r="A6" s="10"/>
       <c r="B6" s="7"/>
-      <c r="C6" s="83"/>
-      <c r="D6" s="83"/>
-      <c r="E6" s="83"/>
-      <c r="F6" s="83"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
       <c r="G6" s="10"/>
       <c r="H6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="73"/>
+      <c r="I6" s="83"/>
       <c r="J6" s="31" t="s">
         <v>80</v>
       </c>
@@ -1599,7 +1611,9 @@
       <c r="W6" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="X6" s="36"/>
+      <c r="X6" s="36" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="7" spans="1:24">
       <c r="A7" s="5" t="s">
@@ -1608,16 +1622,16 @@
       <c r="B7" s="1">
         <v>42948</v>
       </c>
-      <c r="C7" s="81">
+      <c r="C7" s="68">
         <v>12.5</v>
       </c>
-      <c r="D7" s="81">
+      <c r="D7" s="68">
         <v>55</v>
       </c>
-      <c r="E7" s="81">
+      <c r="E7" s="68">
         <v>0.96</v>
       </c>
-      <c r="F7" s="81">
+      <c r="F7" s="68">
         <v>1.19</v>
       </c>
       <c r="G7" s="5" t="s">
@@ -1626,7 +1640,7 @@
       <c r="H7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="68"/>
+      <c r="I7" s="77"/>
       <c r="J7" s="32" t="s">
         <v>80</v>
       </c>
@@ -1652,20 +1666,23 @@
       <c r="W7" s="61" t="s">
         <v>141</v>
       </c>
+      <c r="X7" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="8" spans="1:24">
       <c r="A8" s="5"/>
-      <c r="C8" s="82"/>
-      <c r="D8" s="82"/>
-      <c r="E8" s="82"/>
-      <c r="F8" s="82"/>
+      <c r="C8" s="69"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="69"/>
       <c r="G8" s="5" t="s">
         <v>69</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="69"/>
+      <c r="I8" s="78"/>
       <c r="J8" s="32" t="s">
         <v>80</v>
       </c>
@@ -1691,20 +1708,23 @@
       <c r="W8" s="4" t="s">
         <v>80</v>
       </c>
+      <c r="X8" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="9" spans="1:24">
       <c r="A9" s="5"/>
-      <c r="C9" s="82"/>
-      <c r="D9" s="82"/>
-      <c r="E9" s="82"/>
-      <c r="F9" s="82"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="69"/>
       <c r="G9" s="5" t="s">
         <v>70</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="69"/>
+      <c r="I9" s="78"/>
       <c r="J9" s="32" t="s">
         <v>80</v>
       </c>
@@ -1730,20 +1750,23 @@
       <c r="W9" s="4" t="s">
         <v>80</v>
       </c>
+      <c r="X9" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="10" spans="1:24">
       <c r="A10" s="5"/>
-      <c r="C10" s="82"/>
-      <c r="D10" s="82"/>
-      <c r="E10" s="82"/>
-      <c r="F10" s="82"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
       <c r="G10" s="5" t="s">
         <v>70</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="69"/>
+      <c r="I10" s="78"/>
       <c r="J10" s="32" t="s">
         <v>80</v>
       </c>
@@ -1769,20 +1792,23 @@
       <c r="W10" s="43" t="s">
         <v>139</v>
       </c>
+      <c r="X10" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="11" spans="1:24">
       <c r="A11" s="5"/>
-      <c r="C11" s="82"/>
-      <c r="D11" s="82"/>
-      <c r="E11" s="82"/>
-      <c r="F11" s="82"/>
+      <c r="C11" s="69"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="69"/>
       <c r="G11" s="5" t="s">
         <v>69</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="69"/>
+      <c r="I11" s="78"/>
       <c r="J11" s="32" t="s">
         <v>80</v>
       </c>
@@ -1808,21 +1834,24 @@
       <c r="W11" s="43" t="s">
         <v>139</v>
       </c>
+      <c r="X11" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="12" spans="1:24" s="2" customFormat="1" ht="16" thickBot="1">
       <c r="A12" s="10"/>
       <c r="B12" s="7"/>
-      <c r="C12" s="83"/>
-      <c r="D12" s="83"/>
-      <c r="E12" s="83"/>
-      <c r="F12" s="83"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="70"/>
       <c r="G12" s="10" t="s">
         <v>70</v>
       </c>
       <c r="H12" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="I12" s="70"/>
+      <c r="I12" s="79"/>
       <c r="J12" s="31" t="s">
         <v>80</v>
       </c>
@@ -1849,7 +1878,9 @@
       <c r="W12" s="55" t="s">
         <v>139</v>
       </c>
-      <c r="X12" s="36"/>
+      <c r="X12" s="36" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="13" spans="1:24">
       <c r="A13" s="5" t="s">
@@ -1858,16 +1889,16 @@
       <c r="B13" s="1">
         <v>42956</v>
       </c>
-      <c r="C13" s="81">
+      <c r="C13" s="68">
         <v>16.5</v>
       </c>
-      <c r="D13" s="81">
+      <c r="D13" s="68">
         <v>69</v>
       </c>
-      <c r="E13" s="81">
+      <c r="E13" s="68">
         <v>0.76</v>
       </c>
-      <c r="F13" s="81">
+      <c r="F13" s="68">
         <v>0.87</v>
       </c>
       <c r="G13" s="5" t="s">
@@ -1876,7 +1907,7 @@
       <c r="H13" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="I13" s="68"/>
+      <c r="I13" s="77"/>
       <c r="J13" s="32" t="s">
         <v>80</v>
       </c>
@@ -1902,20 +1933,23 @@
       <c r="W13" s="61" t="s">
         <v>141</v>
       </c>
+      <c r="X13" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="14" spans="1:24">
       <c r="A14" s="5"/>
-      <c r="C14" s="82"/>
-      <c r="D14" s="82"/>
-      <c r="E14" s="82"/>
-      <c r="F14" s="82"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="69"/>
       <c r="G14" s="11" t="s">
         <v>69</v>
       </c>
       <c r="H14" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="I14" s="69"/>
+      <c r="I14" s="78"/>
       <c r="J14" s="32" t="s">
         <v>80</v>
       </c>
@@ -1941,20 +1975,23 @@
       <c r="W14" s="61" t="s">
         <v>141</v>
       </c>
+      <c r="X14" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="15" spans="1:24">
       <c r="A15" s="5"/>
-      <c r="C15" s="82"/>
-      <c r="D15" s="82"/>
-      <c r="E15" s="82"/>
-      <c r="F15" s="82"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="69"/>
       <c r="G15" s="11" t="s">
         <v>69</v>
       </c>
       <c r="H15" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="I15" s="69"/>
+      <c r="I15" s="78"/>
       <c r="J15" s="32" t="s">
         <v>80</v>
       </c>
@@ -1980,20 +2017,23 @@
       <c r="W15" s="4" t="s">
         <v>80</v>
       </c>
+      <c r="X15" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="16" spans="1:24">
       <c r="A16" s="5"/>
-      <c r="C16" s="82"/>
-      <c r="D16" s="82"/>
-      <c r="E16" s="82"/>
-      <c r="F16" s="82"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="69"/>
       <c r="G16" s="11" t="s">
         <v>69</v>
       </c>
       <c r="H16" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="I16" s="69"/>
+      <c r="I16" s="78"/>
       <c r="J16" s="32" t="s">
         <v>80</v>
       </c>
@@ -2019,20 +2059,23 @@
       <c r="W16" s="4" t="s">
         <v>80</v>
       </c>
+      <c r="X16" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="17" spans="1:24">
       <c r="A17" s="5"/>
-      <c r="C17" s="82"/>
-      <c r="D17" s="82"/>
-      <c r="E17" s="82"/>
-      <c r="F17" s="82"/>
+      <c r="C17" s="69"/>
+      <c r="D17" s="69"/>
+      <c r="E17" s="69"/>
+      <c r="F17" s="69"/>
       <c r="G17" s="11" t="s">
         <v>70</v>
       </c>
       <c r="H17" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="I17" s="69"/>
+      <c r="I17" s="78"/>
       <c r="J17" s="32" t="s">
         <v>80</v>
       </c>
@@ -2058,21 +2101,24 @@
       <c r="W17" s="4" t="s">
         <v>80</v>
       </c>
+      <c r="X17" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="18" spans="1:24" s="2" customFormat="1" ht="16" thickBot="1">
       <c r="A18" s="10"/>
       <c r="B18" s="7"/>
-      <c r="C18" s="83"/>
-      <c r="D18" s="83"/>
-      <c r="E18" s="83"/>
-      <c r="F18" s="83"/>
+      <c r="C18" s="70"/>
+      <c r="D18" s="70"/>
+      <c r="E18" s="70"/>
+      <c r="F18" s="70"/>
       <c r="G18" s="10" t="s">
         <v>70</v>
       </c>
       <c r="H18" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="I18" s="70"/>
+      <c r="I18" s="79"/>
       <c r="J18" s="31" t="s">
         <v>80</v>
       </c>
@@ -2099,7 +2145,9 @@
       <c r="W18" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="X18" s="36"/>
+      <c r="X18" s="36" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="19" spans="1:24">
       <c r="A19" s="5" t="s">
@@ -2108,16 +2156,16 @@
       <c r="B19" s="1">
         <v>42971</v>
       </c>
-      <c r="C19" s="81">
+      <c r="C19" s="68">
         <v>16</v>
       </c>
-      <c r="D19" s="81">
+      <c r="D19" s="68">
         <v>70</v>
       </c>
-      <c r="E19" s="81">
+      <c r="E19" s="68">
         <v>0.91</v>
       </c>
-      <c r="F19" s="81">
+      <c r="F19" s="68">
         <v>1.0900000000000001</v>
       </c>
       <c r="G19" s="5" t="s">
@@ -2126,7 +2174,7 @@
       <c r="H19" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="I19" s="71" t="s">
+      <c r="I19" s="81" t="s">
         <v>72</v>
       </c>
       <c r="J19" s="32" t="s">
@@ -2154,20 +2202,23 @@
       <c r="W19" s="61" t="s">
         <v>141</v>
       </c>
+      <c r="X19" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="20" spans="1:24">
       <c r="A20" s="5"/>
-      <c r="C20" s="82"/>
-      <c r="D20" s="82"/>
-      <c r="E20" s="82"/>
-      <c r="F20" s="82"/>
+      <c r="C20" s="69"/>
+      <c r="D20" s="69"/>
+      <c r="E20" s="69"/>
+      <c r="F20" s="69"/>
       <c r="G20" s="11" t="s">
         <v>70</v>
       </c>
       <c r="H20" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="I20" s="72"/>
+      <c r="I20" s="82"/>
       <c r="J20" s="32" t="s">
         <v>80</v>
       </c>
@@ -2193,20 +2244,23 @@
       <c r="W20" s="61" t="s">
         <v>141</v>
       </c>
+      <c r="X20" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="21" spans="1:24">
       <c r="A21" s="5"/>
-      <c r="C21" s="82"/>
-      <c r="D21" s="82"/>
-      <c r="E21" s="82"/>
-      <c r="F21" s="82"/>
+      <c r="C21" s="69"/>
+      <c r="D21" s="69"/>
+      <c r="E21" s="69"/>
+      <c r="F21" s="69"/>
       <c r="G21" s="11" t="s">
         <v>69</v>
       </c>
       <c r="H21" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="I21" s="72"/>
+      <c r="I21" s="82"/>
       <c r="J21" s="32" t="s">
         <v>80</v>
       </c>
@@ -2232,20 +2286,23 @@
       <c r="W21" s="4" t="s">
         <v>80</v>
       </c>
+      <c r="X21" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="22" spans="1:24">
       <c r="A22" s="5"/>
-      <c r="C22" s="82"/>
-      <c r="D22" s="82"/>
-      <c r="E22" s="82"/>
-      <c r="F22" s="82"/>
+      <c r="C22" s="69"/>
+      <c r="D22" s="69"/>
+      <c r="E22" s="69"/>
+      <c r="F22" s="69"/>
       <c r="G22" s="5" t="s">
         <v>69</v>
       </c>
       <c r="H22" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="I22" s="72"/>
+      <c r="I22" s="82"/>
       <c r="J22" s="32" t="s">
         <v>80</v>
       </c>
@@ -2271,20 +2328,23 @@
       <c r="W22" s="4" t="s">
         <v>139</v>
       </c>
+      <c r="X22" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="23" spans="1:24">
       <c r="A23" s="5"/>
-      <c r="C23" s="82"/>
-      <c r="D23" s="82"/>
-      <c r="E23" s="82"/>
-      <c r="F23" s="82"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="69"/>
+      <c r="E23" s="69"/>
+      <c r="F23" s="69"/>
       <c r="G23" s="11" t="s">
         <v>69</v>
       </c>
       <c r="H23" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="I23" s="72"/>
+      <c r="I23" s="82"/>
       <c r="J23" s="32" t="s">
         <v>80</v>
       </c>
@@ -2310,21 +2370,24 @@
       <c r="W23" s="61" t="s">
         <v>141</v>
       </c>
+      <c r="X23" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="24" spans="1:24" s="2" customFormat="1" ht="16" thickBot="1">
       <c r="A24" s="10"/>
       <c r="B24" s="7"/>
-      <c r="C24" s="83"/>
-      <c r="D24" s="83"/>
-      <c r="E24" s="83"/>
-      <c r="F24" s="83"/>
+      <c r="C24" s="70"/>
+      <c r="D24" s="70"/>
+      <c r="E24" s="70"/>
+      <c r="F24" s="70"/>
       <c r="G24" s="10" t="s">
         <v>70</v>
       </c>
       <c r="H24" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="I24" s="73"/>
+      <c r="I24" s="83"/>
       <c r="J24" s="17" t="s">
         <v>79</v>
       </c>
@@ -2344,7 +2407,9 @@
       <c r="P24" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="Q24" s="36"/>
+      <c r="Q24" s="36" t="s">
+        <v>80</v>
+      </c>
       <c r="R24" s="31" t="s">
         <v>80</v>
       </c>
@@ -2361,7 +2426,9 @@
       <c r="W24" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="X24" s="36"/>
+      <c r="X24" s="36" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="25" spans="1:24">
       <c r="A25" s="5" t="s">
@@ -2370,16 +2437,16 @@
       <c r="B25" s="1">
         <v>42969</v>
       </c>
-      <c r="C25" s="81">
+      <c r="C25" s="68">
         <v>19.5</v>
       </c>
-      <c r="D25" s="81">
+      <c r="D25" s="68">
         <v>69</v>
       </c>
-      <c r="E25" s="81">
+      <c r="E25" s="68">
         <v>0.78</v>
       </c>
-      <c r="F25" s="81">
+      <c r="F25" s="68">
         <v>0.96</v>
       </c>
       <c r="G25" s="5" t="s">
@@ -2388,7 +2455,7 @@
       <c r="H25" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="I25" s="68"/>
+      <c r="I25" s="77"/>
       <c r="J25" s="32" t="s">
         <v>80</v>
       </c>
@@ -2414,20 +2481,23 @@
       <c r="W25" s="4" t="s">
         <v>80</v>
       </c>
+      <c r="X25" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="26" spans="1:24">
       <c r="A26" s="5"/>
-      <c r="C26" s="82"/>
-      <c r="D26" s="82"/>
-      <c r="E26" s="82"/>
-      <c r="F26" s="82"/>
+      <c r="C26" s="69"/>
+      <c r="D26" s="69"/>
+      <c r="E26" s="69"/>
+      <c r="F26" s="69"/>
       <c r="G26" s="11" t="s">
         <v>69</v>
       </c>
       <c r="H26" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="I26" s="69"/>
+      <c r="I26" s="78"/>
       <c r="J26" s="32" t="s">
         <v>80</v>
       </c>
@@ -2453,20 +2523,23 @@
       <c r="W26" s="4" t="s">
         <v>80</v>
       </c>
+      <c r="X26" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="27" spans="1:24">
       <c r="A27" s="5"/>
-      <c r="C27" s="82"/>
-      <c r="D27" s="82"/>
-      <c r="E27" s="82"/>
-      <c r="F27" s="82"/>
+      <c r="C27" s="69"/>
+      <c r="D27" s="69"/>
+      <c r="E27" s="69"/>
+      <c r="F27" s="69"/>
       <c r="G27" s="11" t="s">
         <v>69</v>
       </c>
       <c r="H27" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="I27" s="69"/>
+      <c r="I27" s="78"/>
       <c r="J27" s="32" t="s">
         <v>80</v>
       </c>
@@ -2492,20 +2565,23 @@
       <c r="W27" s="4" t="s">
         <v>80</v>
       </c>
+      <c r="X27" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="28" spans="1:24">
       <c r="A28" s="5"/>
-      <c r="C28" s="82"/>
-      <c r="D28" s="82"/>
-      <c r="E28" s="82"/>
-      <c r="F28" s="82"/>
+      <c r="C28" s="69"/>
+      <c r="D28" s="69"/>
+      <c r="E28" s="69"/>
+      <c r="F28" s="69"/>
       <c r="G28" s="11" t="s">
         <v>70</v>
       </c>
       <c r="H28" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="I28" s="69"/>
+      <c r="I28" s="78"/>
       <c r="J28" s="32" t="s">
         <v>80</v>
       </c>
@@ -2531,20 +2607,23 @@
       <c r="W28" s="4" t="s">
         <v>80</v>
       </c>
+      <c r="X28" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="29" spans="1:24">
       <c r="A29" s="5"/>
-      <c r="C29" s="82"/>
-      <c r="D29" s="82"/>
-      <c r="E29" s="82"/>
-      <c r="F29" s="82"/>
+      <c r="C29" s="69"/>
+      <c r="D29" s="69"/>
+      <c r="E29" s="69"/>
+      <c r="F29" s="69"/>
       <c r="G29" s="11" t="s">
         <v>70</v>
       </c>
       <c r="H29" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="I29" s="69"/>
+      <c r="I29" s="78"/>
       <c r="J29" s="32" t="s">
         <v>80</v>
       </c>
@@ -2570,21 +2649,24 @@
       <c r="W29" s="4" t="s">
         <v>80</v>
       </c>
+      <c r="X29" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="30" spans="1:24" s="2" customFormat="1" ht="16" thickBot="1">
       <c r="A30" s="10"/>
       <c r="B30" s="7"/>
-      <c r="C30" s="83"/>
-      <c r="D30" s="83"/>
-      <c r="E30" s="83"/>
-      <c r="F30" s="83"/>
+      <c r="C30" s="70"/>
+      <c r="D30" s="70"/>
+      <c r="E30" s="70"/>
+      <c r="F30" s="70"/>
       <c r="G30" s="10" t="s">
         <v>70</v>
       </c>
       <c r="H30" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="I30" s="70"/>
+      <c r="I30" s="79"/>
       <c r="J30" s="32" t="s">
         <v>80</v>
       </c>
@@ -2611,7 +2693,9 @@
       <c r="W30" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="X30" s="36"/>
+      <c r="X30" s="36" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="31" spans="1:24">
       <c r="A31" s="5" t="s">
@@ -2620,16 +2704,16 @@
       <c r="B31" s="1">
         <v>42978</v>
       </c>
-      <c r="C31" s="81">
+      <c r="C31" s="68">
         <v>17</v>
       </c>
-      <c r="D31" s="81">
+      <c r="D31" s="68">
         <v>69</v>
       </c>
-      <c r="E31" s="81">
+      <c r="E31" s="68">
         <v>0.65</v>
       </c>
-      <c r="F31" s="81">
+      <c r="F31" s="68">
         <v>0.84</v>
       </c>
       <c r="G31" s="5" t="s">
@@ -2638,7 +2722,7 @@
       <c r="H31" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I31" s="68"/>
+      <c r="I31" s="77"/>
       <c r="J31" s="18" t="s">
         <v>79</v>
       </c>
@@ -2655,8 +2739,12 @@
       <c r="O31" s="60" t="s">
         <v>140</v>
       </c>
-      <c r="P31" s="52"/>
-      <c r="Q31" s="62"/>
+      <c r="P31" s="52" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q31" s="62" t="s">
+        <v>80</v>
+      </c>
       <c r="R31" s="32" t="s">
         <v>80</v>
       </c>
@@ -2670,22 +2758,25 @@
         <v>80</v>
       </c>
       <c r="W31" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="X31" s="4" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:24">
       <c r="A32" s="5"/>
-      <c r="C32" s="82"/>
-      <c r="D32" s="82"/>
-      <c r="E32" s="82"/>
-      <c r="F32" s="82"/>
+      <c r="C32" s="69"/>
+      <c r="D32" s="69"/>
+      <c r="E32" s="69"/>
+      <c r="F32" s="69"/>
       <c r="G32" s="11" t="s">
         <v>69</v>
       </c>
       <c r="H32" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="I32" s="69"/>
+      <c r="I32" s="78"/>
       <c r="J32" s="32" t="s">
         <v>80</v>
       </c>
@@ -2711,20 +2802,23 @@
       <c r="W32" s="4" t="s">
         <v>80</v>
       </c>
+      <c r="X32" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="33" spans="1:24">
       <c r="A33" s="5"/>
-      <c r="C33" s="82"/>
-      <c r="D33" s="82"/>
-      <c r="E33" s="82"/>
-      <c r="F33" s="82"/>
+      <c r="C33" s="69"/>
+      <c r="D33" s="69"/>
+      <c r="E33" s="69"/>
+      <c r="F33" s="69"/>
       <c r="G33" s="11" t="s">
         <v>69</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I33" s="69"/>
+      <c r="I33" s="78"/>
       <c r="J33" s="32" t="s">
         <v>80</v>
       </c>
@@ -2750,20 +2844,23 @@
       <c r="W33" s="43" t="s">
         <v>139</v>
       </c>
+      <c r="X33" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="34" spans="1:24">
       <c r="A34" s="5"/>
-      <c r="C34" s="82"/>
-      <c r="D34" s="82"/>
-      <c r="E34" s="82"/>
-      <c r="F34" s="82"/>
+      <c r="C34" s="69"/>
+      <c r="D34" s="69"/>
+      <c r="E34" s="69"/>
+      <c r="F34" s="69"/>
       <c r="G34" s="11" t="s">
         <v>70</v>
       </c>
       <c r="H34" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="I34" s="69"/>
+      <c r="I34" s="78"/>
       <c r="J34" s="18" t="s">
         <v>79</v>
       </c>
@@ -2783,7 +2880,9 @@
       <c r="P34" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="Q34" s="53"/>
+      <c r="Q34" s="53" t="s">
+        <v>80</v>
+      </c>
       <c r="R34" s="32" t="s">
         <v>80</v>
       </c>
@@ -2799,20 +2898,23 @@
       <c r="W34" s="64" t="s">
         <v>139</v>
       </c>
+      <c r="X34" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="35" spans="1:24">
       <c r="A35" s="5"/>
-      <c r="C35" s="82"/>
-      <c r="D35" s="82"/>
-      <c r="E35" s="82"/>
-      <c r="F35" s="82"/>
+      <c r="C35" s="69"/>
+      <c r="D35" s="69"/>
+      <c r="E35" s="69"/>
+      <c r="F35" s="69"/>
       <c r="G35" s="11" t="s">
         <v>70</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="I35" s="69"/>
+      <c r="I35" s="78"/>
       <c r="J35" s="18" t="s">
         <v>79</v>
       </c>
@@ -2832,7 +2934,9 @@
       <c r="P35" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="Q35" s="53"/>
+      <c r="Q35" s="53" t="s">
+        <v>80</v>
+      </c>
       <c r="R35" s="32" t="s">
         <v>80</v>
       </c>
@@ -2847,22 +2951,25 @@
       </c>
       <c r="W35" s="43" t="s">
         <v>139</v>
+      </c>
+      <c r="X35" s="4" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:24" s="2" customFormat="1" ht="16" thickBot="1">
       <c r="A36" s="10"/>
       <c r="B36" s="7"/>
-      <c r="C36" s="83"/>
-      <c r="D36" s="83"/>
-      <c r="E36" s="83"/>
-      <c r="F36" s="83"/>
+      <c r="C36" s="70"/>
+      <c r="D36" s="70"/>
+      <c r="E36" s="70"/>
+      <c r="F36" s="70"/>
       <c r="G36" s="10" t="s">
         <v>70</v>
       </c>
       <c r="H36" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="I36" s="70"/>
+      <c r="I36" s="79"/>
       <c r="J36" s="17" t="s">
         <v>79</v>
       </c>
@@ -2882,7 +2989,9 @@
       <c r="P36" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="Q36" s="36"/>
+      <c r="Q36" s="36" t="s">
+        <v>80</v>
+      </c>
       <c r="R36" s="31" t="s">
         <v>80</v>
       </c>
@@ -2899,7 +3008,9 @@
       <c r="W36" s="55" t="s">
         <v>139</v>
       </c>
-      <c r="X36" s="36"/>
+      <c r="X36" s="36" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="37" spans="1:24">
       <c r="A37" s="5" t="s">
@@ -2908,16 +3019,16 @@
       <c r="B37" s="1">
         <v>42983</v>
       </c>
-      <c r="C37" s="81">
+      <c r="C37" s="68">
         <v>18.5</v>
       </c>
-      <c r="D37" s="81">
+      <c r="D37" s="68">
         <v>82</v>
       </c>
-      <c r="E37" s="81">
+      <c r="E37" s="68">
         <v>0.64</v>
       </c>
-      <c r="F37" s="81">
+      <c r="F37" s="68">
         <v>0.69</v>
       </c>
       <c r="G37" s="5" t="s">
@@ -2926,7 +3037,7 @@
       <c r="H37" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="I37" s="68"/>
+      <c r="I37" s="77"/>
       <c r="J37" s="32" t="s">
         <v>80</v>
       </c>
@@ -2952,20 +3063,23 @@
       <c r="W37" s="64" t="s">
         <v>142</v>
       </c>
+      <c r="X37" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="38" spans="1:24">
       <c r="A38" s="5"/>
-      <c r="C38" s="82"/>
-      <c r="D38" s="82"/>
-      <c r="E38" s="82"/>
-      <c r="F38" s="82"/>
+      <c r="C38" s="69"/>
+      <c r="D38" s="69"/>
+      <c r="E38" s="69"/>
+      <c r="F38" s="69"/>
       <c r="G38" s="11" t="s">
         <v>69</v>
       </c>
       <c r="H38" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="I38" s="69"/>
+      <c r="I38" s="78"/>
       <c r="J38" s="32" t="s">
         <v>80</v>
       </c>
@@ -2991,20 +3105,23 @@
       <c r="W38" s="4" t="s">
         <v>80</v>
       </c>
+      <c r="X38" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="39" spans="1:24">
       <c r="A39" s="5"/>
-      <c r="C39" s="82"/>
-      <c r="D39" s="82"/>
-      <c r="E39" s="82"/>
-      <c r="F39" s="82"/>
+      <c r="C39" s="69"/>
+      <c r="D39" s="69"/>
+      <c r="E39" s="69"/>
+      <c r="F39" s="69"/>
       <c r="G39" s="11" t="s">
         <v>69</v>
       </c>
       <c r="H39" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="I39" s="69"/>
+      <c r="I39" s="78"/>
       <c r="J39" s="32" t="s">
         <v>80</v>
       </c>
@@ -3030,20 +3147,23 @@
       <c r="W39" s="4" t="s">
         <v>80</v>
       </c>
+      <c r="X39" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="40" spans="1:24">
       <c r="A40" s="5"/>
-      <c r="C40" s="82"/>
-      <c r="D40" s="82"/>
-      <c r="E40" s="82"/>
-      <c r="F40" s="82"/>
+      <c r="C40" s="69"/>
+      <c r="D40" s="69"/>
+      <c r="E40" s="69"/>
+      <c r="F40" s="69"/>
       <c r="G40" s="11" t="s">
         <v>70</v>
       </c>
       <c r="H40" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="I40" s="69"/>
+      <c r="I40" s="78"/>
       <c r="J40" s="18" t="s">
         <v>79</v>
       </c>
@@ -3063,7 +3183,9 @@
       <c r="P40" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="Q40" s="53"/>
+      <c r="Q40" s="53" t="s">
+        <v>80</v>
+      </c>
       <c r="R40" s="32" t="s">
         <v>80</v>
       </c>
@@ -3079,20 +3201,23 @@
       <c r="W40" s="64" t="s">
         <v>143</v>
       </c>
+      <c r="X40" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="41" spans="1:24">
       <c r="A41" s="5"/>
-      <c r="C41" s="82"/>
-      <c r="D41" s="82"/>
-      <c r="E41" s="82"/>
-      <c r="F41" s="82"/>
+      <c r="C41" s="69"/>
+      <c r="D41" s="69"/>
+      <c r="E41" s="69"/>
+      <c r="F41" s="69"/>
       <c r="G41" s="11" t="s">
         <v>70</v>
       </c>
       <c r="H41" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="I41" s="69"/>
+      <c r="I41" s="78"/>
       <c r="J41" s="18" t="s">
         <v>79</v>
       </c>
@@ -3112,7 +3237,9 @@
       <c r="P41" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="Q41" s="51"/>
+      <c r="Q41" s="51" t="s">
+        <v>80</v>
+      </c>
       <c r="R41" s="32" t="s">
         <v>80</v>
       </c>
@@ -3127,22 +3254,25 @@
       </c>
       <c r="W41" s="43" t="s">
         <v>139</v>
+      </c>
+      <c r="X41" s="4" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:24" s="2" customFormat="1" ht="16" thickBot="1">
       <c r="A42" s="10"/>
       <c r="B42" s="7"/>
-      <c r="C42" s="83"/>
-      <c r="D42" s="83"/>
-      <c r="E42" s="83"/>
-      <c r="F42" s="83"/>
+      <c r="C42" s="70"/>
+      <c r="D42" s="70"/>
+      <c r="E42" s="70"/>
+      <c r="F42" s="70"/>
       <c r="G42" s="10" t="s">
         <v>70</v>
       </c>
       <c r="H42" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="I42" s="70"/>
+      <c r="I42" s="79"/>
       <c r="J42" s="17" t="s">
         <v>79</v>
       </c>
@@ -3162,7 +3292,9 @@
       <c r="P42" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="Q42" s="44"/>
+      <c r="Q42" s="44" t="s">
+        <v>80</v>
+      </c>
       <c r="R42" s="31" t="s">
         <v>80</v>
       </c>
@@ -3179,7 +3311,9 @@
       <c r="W42" s="63" t="s">
         <v>141</v>
       </c>
-      <c r="X42" s="36"/>
+      <c r="X42" s="36" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="43" spans="1:24">
       <c r="A43" s="5" t="s">
@@ -3188,16 +3322,16 @@
       <c r="B43" s="1">
         <v>42985</v>
       </c>
-      <c r="C43" s="81">
+      <c r="C43" s="68">
         <v>13</v>
       </c>
-      <c r="D43" s="81">
+      <c r="D43" s="68">
         <v>53</v>
       </c>
-      <c r="E43" s="81">
+      <c r="E43" s="68">
         <v>0.64</v>
       </c>
-      <c r="F43" s="81">
+      <c r="F43" s="68">
         <v>0.68</v>
       </c>
       <c r="G43" s="5" t="s">
@@ -3206,7 +3340,7 @@
       <c r="H43" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="I43" s="68"/>
+      <c r="I43" s="77"/>
       <c r="J43" s="32" t="s">
         <v>80</v>
       </c>
@@ -3232,20 +3366,23 @@
       <c r="W43" s="61" t="s">
         <v>141</v>
       </c>
+      <c r="X43" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="44" spans="1:24">
       <c r="A44" s="5"/>
-      <c r="C44" s="82"/>
-      <c r="D44" s="82"/>
-      <c r="E44" s="82"/>
-      <c r="F44" s="82"/>
+      <c r="C44" s="69"/>
+      <c r="D44" s="69"/>
+      <c r="E44" s="69"/>
+      <c r="F44" s="69"/>
       <c r="G44" s="11" t="s">
         <v>69</v>
       </c>
       <c r="H44" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="I44" s="69"/>
+      <c r="I44" s="78"/>
       <c r="J44" s="32" t="s">
         <v>80</v>
       </c>
@@ -3271,20 +3408,23 @@
       <c r="W44" s="64" t="s">
         <v>141</v>
       </c>
+      <c r="X44" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="45" spans="1:24">
       <c r="A45" s="5"/>
-      <c r="C45" s="82"/>
-      <c r="D45" s="82"/>
-      <c r="E45" s="82"/>
-      <c r="F45" s="82"/>
+      <c r="C45" s="69"/>
+      <c r="D45" s="69"/>
+      <c r="E45" s="69"/>
+      <c r="F45" s="69"/>
       <c r="G45" s="11" t="s">
         <v>69</v>
       </c>
       <c r="H45" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="I45" s="69"/>
+      <c r="I45" s="78"/>
       <c r="J45" s="32" t="s">
         <v>80</v>
       </c>
@@ -3310,20 +3450,23 @@
       <c r="W45" s="4" t="s">
         <v>80</v>
       </c>
+      <c r="X45" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="46" spans="1:24">
       <c r="A46" s="5"/>
-      <c r="C46" s="82"/>
-      <c r="D46" s="82"/>
-      <c r="E46" s="82"/>
-      <c r="F46" s="82"/>
+      <c r="C46" s="69"/>
+      <c r="D46" s="69"/>
+      <c r="E46" s="69"/>
+      <c r="F46" s="69"/>
       <c r="G46" s="11" t="s">
         <v>70</v>
       </c>
       <c r="H46" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="I46" s="69"/>
+      <c r="I46" s="78"/>
       <c r="J46" s="18" t="s">
         <v>79</v>
       </c>
@@ -3343,7 +3486,9 @@
       <c r="P46" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="Q46" s="53"/>
+      <c r="Q46" s="53" t="s">
+        <v>80</v>
+      </c>
       <c r="R46" s="32" t="s">
         <v>80</v>
       </c>
@@ -3359,20 +3504,23 @@
       <c r="W46" s="43" t="s">
         <v>139</v>
       </c>
+      <c r="X46" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="47" spans="1:24">
       <c r="A47" s="5"/>
-      <c r="C47" s="82"/>
-      <c r="D47" s="82"/>
-      <c r="E47" s="82"/>
-      <c r="F47" s="82"/>
+      <c r="C47" s="69"/>
+      <c r="D47" s="69"/>
+      <c r="E47" s="69"/>
+      <c r="F47" s="69"/>
       <c r="G47" s="11" t="s">
         <v>70</v>
       </c>
       <c r="H47" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="I47" s="69"/>
+      <c r="I47" s="78"/>
       <c r="J47" s="18" t="s">
         <v>79</v>
       </c>
@@ -3392,7 +3540,9 @@
       <c r="P47" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="Q47" s="53"/>
+      <c r="Q47" s="53" t="s">
+        <v>80</v>
+      </c>
       <c r="R47" s="32" t="s">
         <v>80</v>
       </c>
@@ -3407,22 +3557,25 @@
       </c>
       <c r="W47" s="64" t="s">
         <v>139</v>
+      </c>
+      <c r="X47" s="4" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="48" spans="1:24" s="2" customFormat="1" ht="16" thickBot="1">
       <c r="A48" s="10"/>
       <c r="B48" s="7"/>
-      <c r="C48" s="83"/>
-      <c r="D48" s="83"/>
-      <c r="E48" s="83"/>
-      <c r="F48" s="83"/>
+      <c r="C48" s="70"/>
+      <c r="D48" s="70"/>
+      <c r="E48" s="70"/>
+      <c r="F48" s="70"/>
       <c r="G48" s="10" t="s">
         <v>70</v>
       </c>
       <c r="H48" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="I48" s="70"/>
+      <c r="I48" s="79"/>
       <c r="J48" s="17" t="s">
         <v>79</v>
       </c>
@@ -3442,7 +3595,9 @@
       <c r="P48" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="Q48" s="36"/>
+      <c r="Q48" s="36" t="s">
+        <v>80</v>
+      </c>
       <c r="R48" s="31" t="s">
         <v>80</v>
       </c>
@@ -3459,7 +3614,9 @@
       <c r="W48" s="55" t="s">
         <v>139</v>
       </c>
-      <c r="X48" s="36"/>
+      <c r="X48" s="36" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="49" spans="1:24">
       <c r="A49" s="5" t="s">
@@ -3468,16 +3625,16 @@
       <c r="B49" s="1">
         <v>42992</v>
       </c>
-      <c r="C49" s="81">
+      <c r="C49" s="68">
         <v>16.5</v>
       </c>
-      <c r="D49" s="81">
+      <c r="D49" s="68">
         <v>48</v>
       </c>
-      <c r="E49" s="81">
+      <c r="E49" s="68">
         <v>0.96</v>
       </c>
-      <c r="F49" s="81">
+      <c r="F49" s="68">
         <v>0.99</v>
       </c>
       <c r="G49" s="5" t="s">
@@ -3486,7 +3643,7 @@
       <c r="H49" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="I49" s="68"/>
+      <c r="I49" s="77"/>
       <c r="J49" s="18" t="s">
         <v>79</v>
       </c>
@@ -3506,7 +3663,9 @@
       <c r="P49" s="52" t="s">
         <v>80</v>
       </c>
-      <c r="Q49" s="62"/>
+      <c r="Q49" s="62" t="s">
+        <v>80</v>
+      </c>
       <c r="R49" s="32" t="s">
         <v>80</v>
       </c>
@@ -3520,15 +3679,18 @@
         <v>80</v>
       </c>
       <c r="W49" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="X49" s="4" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="50" spans="1:24">
       <c r="A50" s="5"/>
-      <c r="C50" s="82"/>
-      <c r="D50" s="82"/>
-      <c r="E50" s="82"/>
-      <c r="F50" s="82"/>
+      <c r="C50" s="69"/>
+      <c r="D50" s="69"/>
+      <c r="E50" s="69"/>
+      <c r="F50" s="69"/>
       <c r="G50" s="11" t="s">
         <v>69</v>
       </c>
@@ -3561,13 +3723,16 @@
       <c r="W50" s="43" t="s">
         <v>139</v>
       </c>
+      <c r="X50" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="51" spans="1:24">
       <c r="A51" s="5"/>
-      <c r="C51" s="82"/>
-      <c r="D51" s="82"/>
-      <c r="E51" s="82"/>
-      <c r="F51" s="82"/>
+      <c r="C51" s="69"/>
+      <c r="D51" s="69"/>
+      <c r="E51" s="69"/>
+      <c r="F51" s="69"/>
       <c r="G51" s="11" t="s">
         <v>69</v>
       </c>
@@ -3600,13 +3765,16 @@
       <c r="W51" s="4" t="s">
         <v>80</v>
       </c>
+      <c r="X51" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="52" spans="1:24">
       <c r="A52" s="5"/>
-      <c r="C52" s="82"/>
-      <c r="D52" s="82"/>
-      <c r="E52" s="82"/>
-      <c r="F52" s="82"/>
+      <c r="C52" s="69"/>
+      <c r="D52" s="69"/>
+      <c r="E52" s="69"/>
+      <c r="F52" s="69"/>
       <c r="G52" s="11" t="s">
         <v>70</v>
       </c>
@@ -3633,7 +3801,9 @@
       <c r="P52" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="Q52" s="53"/>
+      <c r="Q52" s="53" t="s">
+        <v>80</v>
+      </c>
       <c r="R52" s="32" t="s">
         <v>80</v>
       </c>
@@ -3649,13 +3819,16 @@
       <c r="W52" s="43" t="s">
         <v>139</v>
       </c>
+      <c r="X52" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="53" spans="1:24">
       <c r="A53" s="5"/>
-      <c r="C53" s="82"/>
-      <c r="D53" s="82"/>
-      <c r="E53" s="82"/>
-      <c r="F53" s="82"/>
+      <c r="C53" s="69"/>
+      <c r="D53" s="69"/>
+      <c r="E53" s="69"/>
+      <c r="F53" s="69"/>
       <c r="G53" s="11" t="s">
         <v>70</v>
       </c>
@@ -3682,7 +3855,9 @@
       <c r="P53" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="Q53" s="53"/>
+      <c r="Q53" s="53" t="s">
+        <v>80</v>
+      </c>
       <c r="R53" s="32" t="s">
         <v>80</v>
       </c>
@@ -3697,22 +3872,25 @@
       </c>
       <c r="W53" s="43" t="s">
         <v>139</v>
+      </c>
+      <c r="X53" s="4" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="54" spans="1:24" s="2" customFormat="1" ht="16" thickBot="1">
       <c r="A54" s="10"/>
       <c r="B54" s="7"/>
-      <c r="C54" s="83"/>
-      <c r="D54" s="83"/>
-      <c r="E54" s="83"/>
-      <c r="F54" s="83"/>
+      <c r="C54" s="70"/>
+      <c r="D54" s="70"/>
+      <c r="E54" s="70"/>
+      <c r="F54" s="70"/>
       <c r="G54" s="10" t="s">
         <v>70</v>
       </c>
       <c r="H54" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="I54" s="70"/>
+      <c r="I54" s="79"/>
       <c r="J54" s="17" t="s">
         <v>79</v>
       </c>
@@ -3732,7 +3910,9 @@
       <c r="P54" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="Q54" s="36"/>
+      <c r="Q54" s="36" t="s">
+        <v>80</v>
+      </c>
       <c r="R54" s="31" t="s">
         <v>80</v>
       </c>
@@ -3749,7 +3929,9 @@
       <c r="W54" s="55" t="s">
         <v>139</v>
       </c>
-      <c r="X54" s="36"/>
+      <c r="X54" s="36" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="55" spans="1:24" ht="16" thickBot="1"/>
     <row r="56" spans="1:24">
@@ -3758,39 +3940,54 @@
       <c r="E56" s="33"/>
       <c r="F56" s="33"/>
       <c r="G56" s="33"/>
-      <c r="S56" s="74" t="s">
+      <c r="S56" s="71" t="s">
         <v>88</v>
       </c>
-      <c r="T56" s="75"/>
+      <c r="T56" s="72"/>
     </row>
     <row r="57" spans="1:24">
-      <c r="S57" s="76"/>
-      <c r="T57" s="77"/>
+      <c r="S57" s="73"/>
+      <c r="T57" s="74"/>
     </row>
     <row r="58" spans="1:24" ht="45" customHeight="1">
       <c r="C58" s="33"/>
       <c r="D58" s="33"/>
       <c r="E58" s="33"/>
       <c r="F58" s="33"/>
-      <c r="S58" s="76" t="s">
+      <c r="S58" s="73" t="s">
         <v>89</v>
       </c>
-      <c r="T58" s="77"/>
+      <c r="T58" s="74"/>
     </row>
     <row r="59" spans="1:24" ht="16" thickBot="1">
-      <c r="S59" s="78"/>
-      <c r="T59" s="79"/>
+      <c r="S59" s="75"/>
+      <c r="T59" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="C2:C6"/>
-    <mergeCell ref="D2:D6"/>
-    <mergeCell ref="E2:E6"/>
-    <mergeCell ref="F2:F6"/>
-    <mergeCell ref="C7:C12"/>
-    <mergeCell ref="D7:D12"/>
-    <mergeCell ref="E7:E12"/>
-    <mergeCell ref="F7:F12"/>
+    <mergeCell ref="I31:I36"/>
+    <mergeCell ref="I2:I6"/>
+    <mergeCell ref="I7:I12"/>
+    <mergeCell ref="I13:I18"/>
+    <mergeCell ref="I19:I24"/>
+    <mergeCell ref="I25:I30"/>
+    <mergeCell ref="S56:T57"/>
+    <mergeCell ref="S58:T59"/>
+    <mergeCell ref="I37:I42"/>
+    <mergeCell ref="I43:I48"/>
+    <mergeCell ref="I49:I54"/>
+    <mergeCell ref="C49:C54"/>
+    <mergeCell ref="D49:D54"/>
+    <mergeCell ref="E49:E54"/>
+    <mergeCell ref="F49:F54"/>
+    <mergeCell ref="C37:C42"/>
+    <mergeCell ref="D37:D42"/>
+    <mergeCell ref="E37:E42"/>
+    <mergeCell ref="F37:F42"/>
+    <mergeCell ref="C43:C48"/>
+    <mergeCell ref="D43:D48"/>
+    <mergeCell ref="E43:E48"/>
+    <mergeCell ref="F43:F48"/>
     <mergeCell ref="C31:C36"/>
     <mergeCell ref="D31:D36"/>
     <mergeCell ref="E31:E36"/>
@@ -3807,29 +4004,14 @@
     <mergeCell ref="D19:D24"/>
     <mergeCell ref="E19:E24"/>
     <mergeCell ref="F19:F24"/>
-    <mergeCell ref="C49:C54"/>
-    <mergeCell ref="D49:D54"/>
-    <mergeCell ref="E49:E54"/>
-    <mergeCell ref="F49:F54"/>
-    <mergeCell ref="C37:C42"/>
-    <mergeCell ref="D37:D42"/>
-    <mergeCell ref="E37:E42"/>
-    <mergeCell ref="F37:F42"/>
-    <mergeCell ref="C43:C48"/>
-    <mergeCell ref="D43:D48"/>
-    <mergeCell ref="E43:E48"/>
-    <mergeCell ref="F43:F48"/>
-    <mergeCell ref="S56:T57"/>
-    <mergeCell ref="S58:T59"/>
-    <mergeCell ref="I37:I42"/>
-    <mergeCell ref="I43:I48"/>
-    <mergeCell ref="I49:I54"/>
-    <mergeCell ref="I31:I36"/>
-    <mergeCell ref="I2:I6"/>
-    <mergeCell ref="I7:I12"/>
-    <mergeCell ref="I13:I18"/>
-    <mergeCell ref="I19:I24"/>
-    <mergeCell ref="I25:I30"/>
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="D2:D6"/>
+    <mergeCell ref="E2:E6"/>
+    <mergeCell ref="F2:F6"/>
+    <mergeCell ref="C7:C12"/>
+    <mergeCell ref="D7:D12"/>
+    <mergeCell ref="E7:E12"/>
+    <mergeCell ref="F7:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="61" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished Tidying the datasets and managed to combine them together!
</commit_message>
<xml_diff>
--- a/data/watercorp_tanks_qpcr_raw_data.xlsx
+++ b/data/watercorp_tanks_qpcr_raw_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natnatraspberry/Desktop/Working Folder/week4_own_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A48626-EB90-744E-A3F1-607698EE613D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{800D0ED7-C20B-8742-92B2-B49E4B523717}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tanks 2017" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="145">
   <si>
     <t>Label on Tubes</t>
   </si>
@@ -482,12 +482,15 @@
   <si>
     <t>Weird MC</t>
   </si>
+  <si>
+    <t>Replicate</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -963,6 +966,45 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -970,45 +1012,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1293,13 +1296,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:X59"/>
+  <dimension ref="A1:Y59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q50" sqref="Q50"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="115" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="50.5" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="1" customWidth="1"/>
@@ -1307,24 +1310,25 @@
     <col min="4" max="6" width="16" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" customWidth="1"/>
     <col min="8" max="8" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21" customWidth="1"/>
-    <col min="10" max="10" width="36.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="30.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.33203125" style="4" customWidth="1"/>
-    <col min="17" max="17" width="21.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="35.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="35.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="28.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="38.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="20.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="21.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" customWidth="1"/>
+    <col min="10" max="10" width="21" customWidth="1"/>
+    <col min="11" max="11" width="36.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="30.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.33203125" style="4" customWidth="1"/>
+    <col min="18" max="18" width="21.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="35.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="35.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="28.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="38.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="21.5" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="3" customFormat="1" ht="16" thickBot="1">
+    <row r="1" spans="1:25" s="3" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>5</v>
       </c>
@@ -1350,94 +1354,99 @@
         <v>0</v>
       </c>
       <c r="I1" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="L1" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="M1" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="N1" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="O1" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="O1" s="67" t="s">
+      <c r="P1" s="67" t="s">
         <v>75</v>
       </c>
-      <c r="P1" s="15" t="s">
+      <c r="Q1" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="Q1" s="67" t="s">
+      <c r="R1" s="67" t="s">
         <v>78</v>
       </c>
-      <c r="R1" s="14" t="s">
+      <c r="S1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="T1" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="T1" s="14" t="s">
+      <c r="U1" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="V1" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="V1" s="16" t="s">
+      <c r="W1" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="W1" s="67" t="s">
+      <c r="X1" s="67" t="s">
         <v>75</v>
       </c>
-      <c r="X1" s="67" t="s">
+      <c r="Y1" s="67" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="1">
         <v>42947</v>
       </c>
-      <c r="C2" s="68">
+      <c r="C2" s="81">
         <v>12</v>
       </c>
-      <c r="D2" s="68">
+      <c r="D2" s="81">
         <v>56</v>
       </c>
-      <c r="E2" s="68">
+      <c r="E2" s="81">
         <v>0.56999999999999995</v>
       </c>
-      <c r="F2" s="68">
+      <c r="F2" s="81">
         <v>0.69</v>
       </c>
-      <c r="G2" s="5"/>
+      <c r="G2" s="5" t="s">
+        <v>69</v>
+      </c>
       <c r="H2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="81" t="s">
+      <c r="I2" s="5">
+        <v>1</v>
+      </c>
+      <c r="J2" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="J2" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="K2" s="47"/>
-      <c r="L2" s="48"/>
+      <c r="K2" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="L2" s="47"/>
       <c r="M2" s="48"/>
-      <c r="N2" s="47"/>
+      <c r="N2" s="48"/>
       <c r="O2" s="47"/>
       <c r="P2" s="47"/>
       <c r="Q2" s="47"/>
-      <c r="R2" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S2" s="4" t="s">
+      <c r="R2" s="47"/>
+      <c r="S2" s="32" t="s">
         <v>80</v>
       </c>
       <c r="T2" s="4" t="s">
@@ -1446,38 +1455,43 @@
       <c r="U2" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="W2" s="61" t="s">
+      <c r="V2" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="X2" s="61" t="s">
         <v>141</v>
       </c>
-      <c r="X2" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24">
+      <c r="Y2" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="5"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="5" t="s">
+        <v>69</v>
+      </c>
       <c r="H3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="82"/>
-      <c r="J3" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="K3" s="34"/>
-      <c r="L3" s="35"/>
+      <c r="I3" s="5">
+        <v>2</v>
+      </c>
+      <c r="J3" s="72"/>
+      <c r="K3" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="L3" s="34"/>
       <c r="M3" s="35"/>
-      <c r="N3" s="34"/>
+      <c r="N3" s="35"/>
       <c r="O3" s="34"/>
       <c r="P3" s="34"/>
       <c r="Q3" s="34"/>
-      <c r="R3" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S3" s="4" t="s">
+      <c r="R3" s="34"/>
+      <c r="S3" s="32" t="s">
         <v>80</v>
       </c>
       <c r="T3" s="4" t="s">
@@ -1486,38 +1500,43 @@
       <c r="U3" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="W3" s="61" t="s">
+      <c r="V3" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="X3" s="61" t="s">
         <v>141</v>
       </c>
-      <c r="X3" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24">
+      <c r="Y3" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="5"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="5" t="s">
+        <v>70</v>
+      </c>
       <c r="H4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="82"/>
-      <c r="J4" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="K4" s="34"/>
-      <c r="L4" s="35"/>
+      <c r="I4" s="5">
+        <v>3</v>
+      </c>
+      <c r="J4" s="72"/>
+      <c r="K4" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="L4" s="34"/>
       <c r="M4" s="35"/>
-      <c r="N4" s="34"/>
+      <c r="N4" s="35"/>
       <c r="O4" s="34"/>
       <c r="P4" s="34"/>
       <c r="Q4" s="34"/>
-      <c r="R4" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S4" s="4" t="s">
+      <c r="R4" s="34"/>
+      <c r="S4" s="32" t="s">
         <v>80</v>
       </c>
       <c r="T4" s="4" t="s">
@@ -1526,38 +1545,43 @@
       <c r="U4" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="W4" s="4" t="s">
+      <c r="V4" s="4" t="s">
         <v>80</v>
       </c>
       <c r="X4" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="5" spans="1:24">
+      <c r="Y4" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="5"/>
+      <c r="C5" s="82"/>
+      <c r="D5" s="82"/>
+      <c r="E5" s="82"/>
+      <c r="F5" s="82"/>
+      <c r="G5" s="5" t="s">
+        <v>69</v>
+      </c>
       <c r="H5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="82"/>
-      <c r="J5" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="K5" s="34"/>
-      <c r="L5" s="35"/>
+      <c r="I5" s="5">
+        <v>4</v>
+      </c>
+      <c r="J5" s="72"/>
+      <c r="K5" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="L5" s="34"/>
       <c r="M5" s="35"/>
-      <c r="N5" s="34"/>
+      <c r="N5" s="35"/>
       <c r="O5" s="34"/>
       <c r="P5" s="34"/>
       <c r="Q5" s="34"/>
-      <c r="R5" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S5" s="4" t="s">
+      <c r="R5" s="34"/>
+      <c r="S5" s="32" t="s">
         <v>80</v>
       </c>
       <c r="T5" s="4" t="s">
@@ -1566,39 +1590,44 @@
       <c r="U5" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="W5" s="61" t="s">
+      <c r="V5" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="X5" s="61" t="s">
         <v>141</v>
       </c>
-      <c r="X5" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" s="2" customFormat="1" ht="16" thickBot="1">
+      <c r="Y5" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" s="2" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="7"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="70"/>
-      <c r="F6" s="70"/>
-      <c r="G6" s="10"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="83"/>
+      <c r="F6" s="83"/>
+      <c r="G6" s="10" t="s">
+        <v>70</v>
+      </c>
       <c r="H6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="83"/>
-      <c r="J6" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="K6" s="49"/>
-      <c r="L6" s="50"/>
+      <c r="I6" s="10">
+        <v>5</v>
+      </c>
+      <c r="J6" s="73"/>
+      <c r="K6" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="L6" s="49"/>
       <c r="M6" s="50"/>
-      <c r="N6" s="49"/>
+      <c r="N6" s="50"/>
       <c r="O6" s="49"/>
       <c r="P6" s="49"/>
       <c r="Q6" s="49"/>
-      <c r="R6" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="S6" s="36" t="s">
+      <c r="R6" s="49"/>
+      <c r="S6" s="31" t="s">
         <v>80</v>
       </c>
       <c r="T6" s="36" t="s">
@@ -1607,31 +1636,34 @@
       <c r="U6" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="V6" s="36"/>
-      <c r="W6" s="36" t="s">
-        <v>80</v>
-      </c>
+      <c r="V6" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="W6" s="36"/>
       <c r="X6" s="36" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="7" spans="1:24">
+      <c r="Y6" s="36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>133</v>
       </c>
       <c r="B7" s="1">
         <v>42948</v>
       </c>
-      <c r="C7" s="68">
+      <c r="C7" s="81">
         <v>12.5</v>
       </c>
-      <c r="D7" s="68">
+      <c r="D7" s="81">
         <v>55</v>
       </c>
-      <c r="E7" s="68">
+      <c r="E7" s="81">
         <v>0.96</v>
       </c>
-      <c r="F7" s="68">
+      <c r="F7" s="81">
         <v>1.19</v>
       </c>
       <c r="G7" s="5" t="s">
@@ -1640,232 +1672,247 @@
       <c r="H7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="77"/>
-      <c r="J7" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="K7" s="34"/>
-      <c r="L7" s="35"/>
+      <c r="I7" s="11">
+        <v>1</v>
+      </c>
+      <c r="J7" s="68"/>
+      <c r="K7" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="L7" s="34"/>
       <c r="M7" s="35"/>
-      <c r="N7" s="34"/>
+      <c r="N7" s="35"/>
       <c r="O7" s="34"/>
       <c r="P7" s="34"/>
       <c r="Q7" s="34"/>
-      <c r="R7" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S7" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="T7" s="51" t="s">
+      <c r="R7" s="34"/>
+      <c r="S7" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="T7" s="4" t="s">
         <v>80</v>
       </c>
       <c r="U7" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="W7" s="61" t="s">
+      <c r="V7" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="X7" s="61" t="s">
         <v>141</v>
       </c>
-      <c r="X7" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24">
+      <c r="Y7" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
-      <c r="C8" s="69"/>
-      <c r="D8" s="69"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="69"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="82"/>
+      <c r="E8" s="82"/>
+      <c r="F8" s="82"/>
       <c r="G8" s="5" t="s">
         <v>69</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="78"/>
-      <c r="J8" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="K8" s="34"/>
-      <c r="L8" s="35"/>
+      <c r="I8" s="11">
+        <v>2</v>
+      </c>
+      <c r="J8" s="69"/>
+      <c r="K8" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="L8" s="34"/>
       <c r="M8" s="35"/>
-      <c r="N8" s="34"/>
+      <c r="N8" s="35"/>
       <c r="O8" s="34"/>
       <c r="P8" s="34"/>
       <c r="Q8" s="34"/>
-      <c r="R8" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S8" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="T8" s="51" t="s">
+      <c r="R8" s="34"/>
+      <c r="S8" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="T8" s="4" t="s">
         <v>80</v>
       </c>
       <c r="U8" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="W8" s="4" t="s">
+      <c r="V8" s="51" t="s">
         <v>80</v>
       </c>
       <c r="X8" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="9" spans="1:24">
+      <c r="Y8" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="69"/>
+      <c r="C9" s="82"/>
+      <c r="D9" s="82"/>
+      <c r="E9" s="82"/>
+      <c r="F9" s="82"/>
       <c r="G9" s="5" t="s">
         <v>70</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="78"/>
-      <c r="J9" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="K9" s="34"/>
-      <c r="L9" s="35"/>
+      <c r="I9" s="11">
+        <v>3</v>
+      </c>
+      <c r="J9" s="69"/>
+      <c r="K9" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="L9" s="34"/>
       <c r="M9" s="35"/>
-      <c r="N9" s="34"/>
+      <c r="N9" s="35"/>
       <c r="O9" s="34"/>
       <c r="P9" s="34"/>
       <c r="Q9" s="34"/>
-      <c r="R9" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S9" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="T9" s="51" t="s">
-        <v>80</v>
-      </c>
-      <c r="U9" s="43" t="s">
+      <c r="R9" s="34"/>
+      <c r="S9" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="T9" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="U9" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="V9" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="W9" s="4" t="s">
-        <v>80</v>
-      </c>
       <c r="X9" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="10" spans="1:24">
+      <c r="Y9" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
-      <c r="C10" s="69"/>
-      <c r="D10" s="69"/>
-      <c r="E10" s="69"/>
-      <c r="F10" s="69"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="82"/>
+      <c r="E10" s="82"/>
+      <c r="F10" s="82"/>
       <c r="G10" s="5" t="s">
         <v>70</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="78"/>
-      <c r="J10" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="K10" s="34"/>
-      <c r="L10" s="35"/>
+      <c r="I10" s="11">
+        <v>4</v>
+      </c>
+      <c r="J10" s="69"/>
+      <c r="K10" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="L10" s="34"/>
       <c r="M10" s="35"/>
-      <c r="N10" s="34"/>
+      <c r="N10" s="35"/>
       <c r="O10" s="34"/>
       <c r="P10" s="34"/>
       <c r="Q10" s="34"/>
-      <c r="R10" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S10" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="T10" s="51" t="s">
-        <v>80</v>
-      </c>
-      <c r="U10" s="43" t="s">
+      <c r="R10" s="34"/>
+      <c r="S10" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="T10" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="U10" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="V10" s="43" t="s">
         <v>127</v>
       </c>
-      <c r="W10" s="43" t="s">
+      <c r="X10" s="43" t="s">
         <v>139</v>
       </c>
-      <c r="X10" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24">
+      <c r="Y10" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="69"/>
+      <c r="C11" s="82"/>
+      <c r="D11" s="82"/>
+      <c r="E11" s="82"/>
+      <c r="F11" s="82"/>
       <c r="G11" s="5" t="s">
         <v>69</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="78"/>
-      <c r="J11" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="K11" s="34"/>
-      <c r="L11" s="35"/>
+      <c r="I11" s="11">
+        <v>5</v>
+      </c>
+      <c r="J11" s="69"/>
+      <c r="K11" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="L11" s="34"/>
       <c r="M11" s="35"/>
-      <c r="N11" s="34"/>
+      <c r="N11" s="35"/>
       <c r="O11" s="34"/>
       <c r="P11" s="34"/>
       <c r="Q11" s="34"/>
-      <c r="R11" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S11" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="T11" s="51" t="s">
-        <v>80</v>
-      </c>
-      <c r="U11" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="W11" s="43" t="s">
+      <c r="R11" s="34"/>
+      <c r="S11" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="T11" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="U11" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="V11" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="X11" s="43" t="s">
         <v>139</v>
       </c>
-      <c r="X11" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" s="2" customFormat="1" ht="16" thickBot="1">
+      <c r="Y11" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" s="2" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="7"/>
-      <c r="C12" s="70"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="70"/>
+      <c r="C12" s="83"/>
+      <c r="D12" s="83"/>
+      <c r="E12" s="83"/>
+      <c r="F12" s="83"/>
       <c r="G12" s="10" t="s">
         <v>70</v>
       </c>
       <c r="H12" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="I12" s="79"/>
-      <c r="J12" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="K12" s="49"/>
-      <c r="L12" s="50"/>
+      <c r="I12" s="10">
+        <v>6</v>
+      </c>
+      <c r="J12" s="70"/>
+      <c r="K12" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="L12" s="49"/>
       <c r="M12" s="50"/>
-      <c r="N12" s="49"/>
+      <c r="N12" s="50"/>
       <c r="O12" s="49"/>
       <c r="P12" s="49"/>
       <c r="Q12" s="49"/>
-      <c r="R12" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="S12" s="36" t="s">
+      <c r="R12" s="49"/>
+      <c r="S12" s="31" t="s">
         <v>80</v>
       </c>
       <c r="T12" s="36" t="s">
@@ -1874,31 +1921,34 @@
       <c r="U12" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="V12" s="36"/>
-      <c r="W12" s="55" t="s">
+      <c r="V12" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="W12" s="36"/>
+      <c r="X12" s="55" t="s">
         <v>139</v>
       </c>
-      <c r="X12" s="36" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24">
+      <c r="Y12" s="36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="1">
         <v>42956</v>
       </c>
-      <c r="C13" s="68">
+      <c r="C13" s="81">
         <v>16.5</v>
       </c>
-      <c r="D13" s="68">
+      <c r="D13" s="81">
         <v>69</v>
       </c>
-      <c r="E13" s="68">
+      <c r="E13" s="81">
         <v>0.76</v>
       </c>
-      <c r="F13" s="68">
+      <c r="F13" s="81">
         <v>0.87</v>
       </c>
       <c r="G13" s="5" t="s">
@@ -1907,232 +1957,247 @@
       <c r="H13" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="I13" s="77"/>
-      <c r="J13" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="K13" s="34"/>
-      <c r="L13" s="35"/>
+      <c r="I13" s="11">
+        <v>1</v>
+      </c>
+      <c r="J13" s="68"/>
+      <c r="K13" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="L13" s="34"/>
       <c r="M13" s="35"/>
-      <c r="N13" s="34"/>
+      <c r="N13" s="35"/>
       <c r="O13" s="34"/>
       <c r="P13" s="34"/>
       <c r="Q13" s="34"/>
-      <c r="R13" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S13" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="T13" s="51" t="s">
+      <c r="R13" s="34"/>
+      <c r="S13" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="T13" s="4" t="s">
         <v>80</v>
       </c>
       <c r="U13" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="W13" s="61" t="s">
+      <c r="V13" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="X13" s="61" t="s">
         <v>141</v>
       </c>
-      <c r="X13" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24">
+      <c r="Y13" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
-      <c r="C14" s="69"/>
-      <c r="D14" s="69"/>
-      <c r="E14" s="69"/>
-      <c r="F14" s="69"/>
+      <c r="C14" s="82"/>
+      <c r="D14" s="82"/>
+      <c r="E14" s="82"/>
+      <c r="F14" s="82"/>
       <c r="G14" s="11" t="s">
         <v>69</v>
       </c>
       <c r="H14" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="I14" s="78"/>
-      <c r="J14" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="K14" s="34"/>
-      <c r="L14" s="35"/>
+      <c r="I14" s="11">
+        <v>2</v>
+      </c>
+      <c r="J14" s="69"/>
+      <c r="K14" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="L14" s="34"/>
       <c r="M14" s="35"/>
-      <c r="N14" s="34"/>
+      <c r="N14" s="35"/>
       <c r="O14" s="34"/>
       <c r="P14" s="34"/>
       <c r="Q14" s="34"/>
-      <c r="R14" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S14" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="T14" s="51" t="s">
+      <c r="R14" s="34"/>
+      <c r="S14" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="T14" s="4" t="s">
         <v>80</v>
       </c>
       <c r="U14" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="W14" s="61" t="s">
+      <c r="V14" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="X14" s="61" t="s">
         <v>141</v>
       </c>
-      <c r="X14" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24">
+      <c r="Y14" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
-      <c r="C15" s="69"/>
-      <c r="D15" s="69"/>
-      <c r="E15" s="69"/>
-      <c r="F15" s="69"/>
+      <c r="C15" s="82"/>
+      <c r="D15" s="82"/>
+      <c r="E15" s="82"/>
+      <c r="F15" s="82"/>
       <c r="G15" s="11" t="s">
         <v>69</v>
       </c>
       <c r="H15" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="I15" s="78"/>
-      <c r="J15" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="K15" s="34"/>
-      <c r="L15" s="35"/>
+      <c r="I15" s="11">
+        <v>3</v>
+      </c>
+      <c r="J15" s="69"/>
+      <c r="K15" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="L15" s="34"/>
       <c r="M15" s="35"/>
-      <c r="N15" s="34"/>
+      <c r="N15" s="35"/>
       <c r="O15" s="34"/>
       <c r="P15" s="34"/>
       <c r="Q15" s="34"/>
-      <c r="R15" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S15" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="T15" s="51" t="s">
+      <c r="R15" s="34"/>
+      <c r="S15" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="T15" s="4" t="s">
         <v>80</v>
       </c>
       <c r="U15" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="W15" s="4" t="s">
+      <c r="V15" s="51" t="s">
         <v>80</v>
       </c>
       <c r="X15" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="16" spans="1:24">
+      <c r="Y15" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
-      <c r="C16" s="69"/>
-      <c r="D16" s="69"/>
-      <c r="E16" s="69"/>
-      <c r="F16" s="69"/>
+      <c r="C16" s="82"/>
+      <c r="D16" s="82"/>
+      <c r="E16" s="82"/>
+      <c r="F16" s="82"/>
       <c r="G16" s="11" t="s">
         <v>69</v>
       </c>
       <c r="H16" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="I16" s="78"/>
-      <c r="J16" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="K16" s="34"/>
-      <c r="L16" s="35"/>
+      <c r="I16" s="11">
+        <v>4</v>
+      </c>
+      <c r="J16" s="69"/>
+      <c r="K16" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="L16" s="34"/>
       <c r="M16" s="35"/>
-      <c r="N16" s="34"/>
+      <c r="N16" s="35"/>
       <c r="O16" s="34"/>
       <c r="P16" s="34"/>
       <c r="Q16" s="34"/>
-      <c r="R16" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S16" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="T16" s="51" t="s">
+      <c r="R16" s="34"/>
+      <c r="S16" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="T16" s="4" t="s">
         <v>80</v>
       </c>
       <c r="U16" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="W16" s="4" t="s">
+      <c r="V16" s="51" t="s">
         <v>80</v>
       </c>
       <c r="X16" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="17" spans="1:24">
+      <c r="Y16" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" s="5"/>
-      <c r="C17" s="69"/>
-      <c r="D17" s="69"/>
-      <c r="E17" s="69"/>
-      <c r="F17" s="69"/>
+      <c r="C17" s="82"/>
+      <c r="D17" s="82"/>
+      <c r="E17" s="82"/>
+      <c r="F17" s="82"/>
       <c r="G17" s="11" t="s">
         <v>70</v>
       </c>
       <c r="H17" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="I17" s="78"/>
-      <c r="J17" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="K17" s="34"/>
-      <c r="L17" s="35"/>
+      <c r="I17" s="11">
+        <v>5</v>
+      </c>
+      <c r="J17" s="69"/>
+      <c r="K17" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="L17" s="34"/>
       <c r="M17" s="35"/>
-      <c r="N17" s="34"/>
+      <c r="N17" s="35"/>
       <c r="O17" s="34"/>
       <c r="P17" s="34"/>
       <c r="Q17" s="34"/>
-      <c r="R17" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S17" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="T17" s="51" t="s">
+      <c r="R17" s="34"/>
+      <c r="S17" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="T17" s="4" t="s">
         <v>80</v>
       </c>
       <c r="U17" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="W17" s="4" t="s">
+      <c r="V17" s="51" t="s">
         <v>80</v>
       </c>
       <c r="X17" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="18" spans="1:24" s="2" customFormat="1" ht="16" thickBot="1">
+      <c r="Y17" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" s="2" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="7"/>
-      <c r="C18" s="70"/>
-      <c r="D18" s="70"/>
-      <c r="E18" s="70"/>
-      <c r="F18" s="70"/>
+      <c r="C18" s="83"/>
+      <c r="D18" s="83"/>
+      <c r="E18" s="83"/>
+      <c r="F18" s="83"/>
       <c r="G18" s="10" t="s">
         <v>70</v>
       </c>
       <c r="H18" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="I18" s="79"/>
-      <c r="J18" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="K18" s="49"/>
-      <c r="L18" s="50"/>
+      <c r="I18" s="12">
+        <v>6</v>
+      </c>
+      <c r="J18" s="70"/>
+      <c r="K18" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="L18" s="49"/>
       <c r="M18" s="50"/>
-      <c r="N18" s="49"/>
+      <c r="N18" s="50"/>
       <c r="O18" s="49"/>
       <c r="P18" s="49"/>
       <c r="Q18" s="49"/>
-      <c r="R18" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="S18" s="36" t="s">
+      <c r="R18" s="49"/>
+      <c r="S18" s="31" t="s">
         <v>80</v>
       </c>
       <c r="T18" s="36" t="s">
@@ -2141,31 +2206,34 @@
       <c r="U18" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="V18" s="36"/>
-      <c r="W18" s="36" t="s">
-        <v>80</v>
-      </c>
+      <c r="V18" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="W18" s="36"/>
       <c r="X18" s="36" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="19" spans="1:24">
+      <c r="Y18" s="36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="1">
         <v>42971</v>
       </c>
-      <c r="C19" s="68">
+      <c r="C19" s="81">
         <v>16</v>
       </c>
-      <c r="D19" s="68">
+      <c r="D19" s="81">
         <v>70</v>
       </c>
-      <c r="E19" s="68">
+      <c r="E19" s="81">
         <v>0.91</v>
       </c>
-      <c r="F19" s="68">
+      <c r="F19" s="81">
         <v>1.0900000000000001</v>
       </c>
       <c r="G19" s="5" t="s">
@@ -2174,279 +2242,297 @@
       <c r="H19" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="I19" s="81" t="s">
+      <c r="I19" s="11">
+        <v>1</v>
+      </c>
+      <c r="J19" s="71" t="s">
         <v>72</v>
       </c>
-      <c r="J19" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="K19" s="34"/>
-      <c r="L19" s="35"/>
+      <c r="K19" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="L19" s="34"/>
       <c r="M19" s="35"/>
-      <c r="N19" s="34"/>
+      <c r="N19" s="35"/>
       <c r="O19" s="34"/>
       <c r="P19" s="34"/>
       <c r="Q19" s="34"/>
-      <c r="R19" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S19" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="T19" s="51" t="s">
+      <c r="R19" s="34"/>
+      <c r="S19" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="T19" s="4" t="s">
         <v>80</v>
       </c>
       <c r="U19" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="W19" s="61" t="s">
+      <c r="V19" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="X19" s="61" t="s">
         <v>141</v>
       </c>
-      <c r="X19" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:24">
+      <c r="Y19" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" s="5"/>
-      <c r="C20" s="69"/>
-      <c r="D20" s="69"/>
-      <c r="E20" s="69"/>
-      <c r="F20" s="69"/>
+      <c r="C20" s="82"/>
+      <c r="D20" s="82"/>
+      <c r="E20" s="82"/>
+      <c r="F20" s="82"/>
       <c r="G20" s="11" t="s">
         <v>70</v>
       </c>
       <c r="H20" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="I20" s="82"/>
-      <c r="J20" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="K20" s="34"/>
-      <c r="L20" s="35"/>
+      <c r="I20" s="11">
+        <v>2</v>
+      </c>
+      <c r="J20" s="72"/>
+      <c r="K20" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="L20" s="34"/>
       <c r="M20" s="35"/>
-      <c r="N20" s="34"/>
+      <c r="N20" s="35"/>
       <c r="O20" s="34"/>
       <c r="P20" s="34"/>
       <c r="Q20" s="34"/>
-      <c r="R20" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S20" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="T20" s="51" t="s">
+      <c r="R20" s="34"/>
+      <c r="S20" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="T20" s="4" t="s">
         <v>80</v>
       </c>
       <c r="U20" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="W20" s="61" t="s">
+      <c r="V20" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="X20" s="61" t="s">
         <v>141</v>
       </c>
-      <c r="X20" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:24">
+      <c r="Y20" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" s="5"/>
-      <c r="C21" s="69"/>
-      <c r="D21" s="69"/>
-      <c r="E21" s="69"/>
-      <c r="F21" s="69"/>
+      <c r="C21" s="82"/>
+      <c r="D21" s="82"/>
+      <c r="E21" s="82"/>
+      <c r="F21" s="82"/>
       <c r="G21" s="11" t="s">
         <v>69</v>
       </c>
       <c r="H21" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="I21" s="82"/>
-      <c r="J21" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="K21" s="34"/>
-      <c r="L21" s="35"/>
+      <c r="I21" s="11">
+        <v>3</v>
+      </c>
+      <c r="J21" s="72"/>
+      <c r="K21" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="L21" s="34"/>
       <c r="M21" s="35"/>
-      <c r="N21" s="34"/>
+      <c r="N21" s="35"/>
       <c r="O21" s="34"/>
       <c r="P21" s="34"/>
       <c r="Q21" s="34"/>
-      <c r="R21" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S21" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="T21" s="51" t="s">
+      <c r="R21" s="34"/>
+      <c r="S21" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="T21" s="4" t="s">
         <v>80</v>
       </c>
       <c r="U21" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="W21" s="4" t="s">
+      <c r="V21" s="51" t="s">
         <v>80</v>
       </c>
       <c r="X21" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="22" spans="1:24">
+      <c r="Y21" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" s="5"/>
-      <c r="C22" s="69"/>
-      <c r="D22" s="69"/>
-      <c r="E22" s="69"/>
-      <c r="F22" s="69"/>
+      <c r="C22" s="82"/>
+      <c r="D22" s="82"/>
+      <c r="E22" s="82"/>
+      <c r="F22" s="82"/>
       <c r="G22" s="5" t="s">
         <v>69</v>
       </c>
       <c r="H22" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="I22" s="82"/>
-      <c r="J22" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="K22" s="34"/>
-      <c r="L22" s="35"/>
+      <c r="I22" s="11">
+        <v>4</v>
+      </c>
+      <c r="J22" s="72"/>
+      <c r="K22" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="L22" s="34"/>
       <c r="M22" s="35"/>
-      <c r="N22" s="34"/>
+      <c r="N22" s="35"/>
       <c r="O22" s="34"/>
       <c r="P22" s="34"/>
       <c r="Q22" s="34"/>
-      <c r="R22" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S22" s="56" t="s">
+      <c r="R22" s="34"/>
+      <c r="S22" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="T22" s="56" t="s">
         <v>138</v>
       </c>
-      <c r="T22" s="51" t="s">
-        <v>80</v>
-      </c>
       <c r="U22" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="W22" s="4" t="s">
+      <c r="V22" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="X22" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="X22" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24">
+      <c r="Y22" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23" s="5"/>
-      <c r="C23" s="69"/>
-      <c r="D23" s="69"/>
-      <c r="E23" s="69"/>
-      <c r="F23" s="69"/>
+      <c r="C23" s="82"/>
+      <c r="D23" s="82"/>
+      <c r="E23" s="82"/>
+      <c r="F23" s="82"/>
       <c r="G23" s="11" t="s">
         <v>69</v>
       </c>
       <c r="H23" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="I23" s="82"/>
-      <c r="J23" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="K23" s="34"/>
-      <c r="L23" s="35"/>
+      <c r="I23" s="11">
+        <v>5</v>
+      </c>
+      <c r="J23" s="72"/>
+      <c r="K23" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="L23" s="34"/>
       <c r="M23" s="35"/>
-      <c r="N23" s="34"/>
+      <c r="N23" s="35"/>
       <c r="O23" s="34"/>
       <c r="P23" s="34"/>
       <c r="Q23" s="34"/>
-      <c r="R23" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S23" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="T23" s="51" t="s">
+      <c r="R23" s="34"/>
+      <c r="S23" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="T23" s="4" t="s">
         <v>80</v>
       </c>
       <c r="U23" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="W23" s="61" t="s">
+      <c r="V23" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="X23" s="61" t="s">
         <v>141</v>
       </c>
-      <c r="X23" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="24" spans="1:24" s="2" customFormat="1" ht="16" thickBot="1">
+      <c r="Y23" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" s="2" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
       <c r="B24" s="7"/>
-      <c r="C24" s="70"/>
-      <c r="D24" s="70"/>
-      <c r="E24" s="70"/>
-      <c r="F24" s="70"/>
+      <c r="C24" s="83"/>
+      <c r="D24" s="83"/>
+      <c r="E24" s="83"/>
+      <c r="F24" s="83"/>
       <c r="G24" s="10" t="s">
         <v>70</v>
       </c>
       <c r="H24" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="I24" s="83"/>
-      <c r="J24" s="17" t="s">
+      <c r="I24" s="12">
+        <v>6</v>
+      </c>
+      <c r="J24" s="73"/>
+      <c r="K24" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="K24" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="L24" s="31" t="s">
+      <c r="L24" s="36" t="s">
         <v>80</v>
       </c>
       <c r="M24" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="N24" s="36"/>
-      <c r="O24" s="44" t="s">
-        <v>80</v>
-      </c>
-      <c r="P24" s="36" t="s">
+      <c r="N24" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="O24" s="36"/>
+      <c r="P24" s="44" t="s">
         <v>80</v>
       </c>
       <c r="Q24" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="R24" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="S24" s="36" t="s">
+      <c r="R24" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="S24" s="31" t="s">
         <v>80</v>
       </c>
       <c r="T24" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="U24" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="V24" s="36"/>
-      <c r="W24" s="36" t="s">
-        <v>80</v>
-      </c>
+      <c r="U24" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="V24" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="W24" s="36"/>
       <c r="X24" s="36" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="25" spans="1:24">
+      <c r="Y24" s="36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B25" s="1">
         <v>42969</v>
       </c>
-      <c r="C25" s="68">
+      <c r="C25" s="81">
         <v>19.5</v>
       </c>
-      <c r="D25" s="68">
+      <c r="D25" s="81">
         <v>69</v>
       </c>
-      <c r="E25" s="68">
+      <c r="E25" s="81">
         <v>0.78</v>
       </c>
-      <c r="F25" s="68">
+      <c r="F25" s="81">
         <v>0.96</v>
       </c>
       <c r="G25" s="5" t="s">
@@ -2455,265 +2541,283 @@
       <c r="H25" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="I25" s="77"/>
-      <c r="J25" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="K25" s="37"/>
-      <c r="L25" s="38"/>
+      <c r="I25" s="11">
+        <v>1</v>
+      </c>
+      <c r="J25" s="68"/>
+      <c r="K25" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="L25" s="37"/>
       <c r="M25" s="38"/>
-      <c r="N25" s="37"/>
+      <c r="N25" s="38"/>
       <c r="O25" s="37"/>
       <c r="P25" s="37"/>
       <c r="Q25" s="37"/>
-      <c r="R25" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S25" s="4" t="s">
+      <c r="R25" s="37"/>
+      <c r="S25" s="32" t="s">
         <v>80</v>
       </c>
       <c r="T25" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="U25" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="W25" s="4" t="s">
+      <c r="U25" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="V25" s="46" t="s">
         <v>80</v>
       </c>
       <c r="X25" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="26" spans="1:24">
+      <c r="Y25" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26" s="5"/>
-      <c r="C26" s="69"/>
-      <c r="D26" s="69"/>
-      <c r="E26" s="69"/>
-      <c r="F26" s="69"/>
+      <c r="C26" s="82"/>
+      <c r="D26" s="82"/>
+      <c r="E26" s="82"/>
+      <c r="F26" s="82"/>
       <c r="G26" s="11" t="s">
         <v>69</v>
       </c>
       <c r="H26" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="I26" s="78"/>
-      <c r="J26" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="K26" s="39"/>
-      <c r="L26" s="40"/>
+      <c r="I26" s="11">
+        <v>2</v>
+      </c>
+      <c r="J26" s="69"/>
+      <c r="K26" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="L26" s="39"/>
       <c r="M26" s="40"/>
-      <c r="N26" s="39"/>
+      <c r="N26" s="40"/>
       <c r="O26" s="39"/>
       <c r="P26" s="39"/>
       <c r="Q26" s="39"/>
-      <c r="R26" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S26" s="4" t="s">
+      <c r="R26" s="39"/>
+      <c r="S26" s="32" t="s">
         <v>80</v>
       </c>
       <c r="T26" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="U26" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="W26" s="4" t="s">
+      <c r="U26" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="V26" s="46" t="s">
         <v>80</v>
       </c>
       <c r="X26" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="27" spans="1:24">
+      <c r="Y26" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27" s="5"/>
-      <c r="C27" s="69"/>
-      <c r="D27" s="69"/>
-      <c r="E27" s="69"/>
-      <c r="F27" s="69"/>
+      <c r="C27" s="82"/>
+      <c r="D27" s="82"/>
+      <c r="E27" s="82"/>
+      <c r="F27" s="82"/>
       <c r="G27" s="11" t="s">
         <v>69</v>
       </c>
       <c r="H27" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="I27" s="78"/>
-      <c r="J27" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="K27" s="39"/>
-      <c r="L27" s="40"/>
+      <c r="I27" s="11">
+        <v>3</v>
+      </c>
+      <c r="J27" s="69"/>
+      <c r="K27" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="L27" s="39"/>
       <c r="M27" s="40"/>
-      <c r="N27" s="39"/>
+      <c r="N27" s="40"/>
       <c r="O27" s="39"/>
       <c r="P27" s="39"/>
       <c r="Q27" s="39"/>
-      <c r="R27" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S27" s="4" t="s">
+      <c r="R27" s="39"/>
+      <c r="S27" s="32" t="s">
         <v>80</v>
       </c>
       <c r="T27" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="U27" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="W27" s="4" t="s">
+      <c r="U27" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="V27" s="46" t="s">
         <v>80</v>
       </c>
       <c r="X27" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="28" spans="1:24">
+      <c r="Y27" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A28" s="5"/>
-      <c r="C28" s="69"/>
-      <c r="D28" s="69"/>
-      <c r="E28" s="69"/>
-      <c r="F28" s="69"/>
+      <c r="C28" s="82"/>
+      <c r="D28" s="82"/>
+      <c r="E28" s="82"/>
+      <c r="F28" s="82"/>
       <c r="G28" s="11" t="s">
         <v>70</v>
       </c>
       <c r="H28" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="I28" s="78"/>
-      <c r="J28" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="K28" s="39"/>
-      <c r="L28" s="40"/>
+      <c r="I28" s="11">
+        <v>4</v>
+      </c>
+      <c r="J28" s="69"/>
+      <c r="K28" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="L28" s="39"/>
       <c r="M28" s="40"/>
-      <c r="N28" s="39"/>
+      <c r="N28" s="40"/>
       <c r="O28" s="39"/>
       <c r="P28" s="39"/>
       <c r="Q28" s="39"/>
-      <c r="R28" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S28" s="4" t="s">
+      <c r="R28" s="39"/>
+      <c r="S28" s="32" t="s">
         <v>80</v>
       </c>
       <c r="T28" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="U28" s="43" t="s">
+      <c r="U28" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="V28" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="W28" s="4" t="s">
-        <v>80</v>
-      </c>
       <c r="X28" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="29" spans="1:24">
+      <c r="Y28" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A29" s="5"/>
-      <c r="C29" s="69"/>
-      <c r="D29" s="69"/>
-      <c r="E29" s="69"/>
-      <c r="F29" s="69"/>
+      <c r="C29" s="82"/>
+      <c r="D29" s="82"/>
+      <c r="E29" s="82"/>
+      <c r="F29" s="82"/>
       <c r="G29" s="11" t="s">
         <v>70</v>
       </c>
       <c r="H29" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="I29" s="78"/>
-      <c r="J29" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="K29" s="39"/>
-      <c r="L29" s="40"/>
+      <c r="I29" s="11">
+        <v>5</v>
+      </c>
+      <c r="J29" s="69"/>
+      <c r="K29" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="L29" s="39"/>
       <c r="M29" s="40"/>
-      <c r="N29" s="39"/>
+      <c r="N29" s="40"/>
       <c r="O29" s="39"/>
       <c r="P29" s="39"/>
       <c r="Q29" s="39"/>
-      <c r="R29" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S29" s="4" t="s">
+      <c r="R29" s="39"/>
+      <c r="S29" s="32" t="s">
         <v>80</v>
       </c>
       <c r="T29" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="U29" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="W29" s="4" t="s">
+      <c r="U29" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="V29" s="30" t="s">
         <v>80</v>
       </c>
       <c r="X29" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="30" spans="1:24" s="2" customFormat="1" ht="16" thickBot="1">
+      <c r="Y29" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" s="2" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10"/>
       <c r="B30" s="7"/>
-      <c r="C30" s="70"/>
-      <c r="D30" s="70"/>
-      <c r="E30" s="70"/>
-      <c r="F30" s="70"/>
+      <c r="C30" s="83"/>
+      <c r="D30" s="83"/>
+      <c r="E30" s="83"/>
+      <c r="F30" s="83"/>
       <c r="G30" s="10" t="s">
         <v>70</v>
       </c>
       <c r="H30" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="I30" s="79"/>
-      <c r="J30" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="K30" s="41"/>
-      <c r="L30" s="42"/>
+      <c r="I30" s="12">
+        <v>6</v>
+      </c>
+      <c r="J30" s="70"/>
+      <c r="K30" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="L30" s="41"/>
       <c r="M30" s="42"/>
-      <c r="N30" s="41"/>
+      <c r="N30" s="42"/>
       <c r="O30" s="41"/>
       <c r="P30" s="41"/>
       <c r="Q30" s="41"/>
-      <c r="R30" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="S30" s="36" t="s">
+      <c r="R30" s="41"/>
+      <c r="S30" s="31" t="s">
         <v>80</v>
       </c>
       <c r="T30" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="U30" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="V30" s="36"/>
-      <c r="W30" s="36" t="s">
-        <v>80</v>
-      </c>
+      <c r="U30" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="V30" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="W30" s="36"/>
       <c r="X30" s="36" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="31" spans="1:24">
+      <c r="Y30" s="36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B31" s="1">
         <v>42978</v>
       </c>
-      <c r="C31" s="68">
+      <c r="C31" s="81">
         <v>17</v>
       </c>
-      <c r="D31" s="68">
+      <c r="D31" s="81">
         <v>69</v>
       </c>
-      <c r="E31" s="68">
+      <c r="E31" s="81">
         <v>0.65</v>
       </c>
-      <c r="F31" s="68">
+      <c r="F31" s="81">
         <v>0.84</v>
       </c>
       <c r="G31" s="5" t="s">
@@ -2722,313 +2826,331 @@
       <c r="H31" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I31" s="77"/>
-      <c r="J31" s="18" t="s">
+      <c r="I31" s="11">
+        <v>1</v>
+      </c>
+      <c r="J31" s="68"/>
+      <c r="K31" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="K31" s="43" t="s">
+      <c r="L31" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="L31" s="4" t="s">
-        <v>80</v>
-      </c>
       <c r="M31" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="N31" s="52"/>
-      <c r="O31" s="60" t="s">
+      <c r="N31" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="O31" s="52"/>
+      <c r="P31" s="60" t="s">
         <v>140</v>
       </c>
-      <c r="P31" s="52" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q31" s="62" t="s">
-        <v>80</v>
-      </c>
-      <c r="R31" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S31" s="51" t="s">
-        <v>80</v>
-      </c>
-      <c r="T31" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="U31" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="W31" s="4" t="s">
+      <c r="Q31" s="52" t="s">
+        <v>80</v>
+      </c>
+      <c r="R31" s="62" t="s">
+        <v>80</v>
+      </c>
+      <c r="S31" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="T31" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="U31" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="V31" s="46" t="s">
         <v>80</v>
       </c>
       <c r="X31" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="32" spans="1:24">
+      <c r="Y31" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A32" s="5"/>
-      <c r="C32" s="69"/>
-      <c r="D32" s="69"/>
-      <c r="E32" s="69"/>
-      <c r="F32" s="69"/>
+      <c r="C32" s="82"/>
+      <c r="D32" s="82"/>
+      <c r="E32" s="82"/>
+      <c r="F32" s="82"/>
       <c r="G32" s="11" t="s">
         <v>69</v>
       </c>
       <c r="H32" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="I32" s="78"/>
-      <c r="J32" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="K32" s="39"/>
-      <c r="L32" s="40"/>
+      <c r="I32" s="11">
+        <v>2</v>
+      </c>
+      <c r="J32" s="69"/>
+      <c r="K32" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="L32" s="39"/>
       <c r="M32" s="40"/>
-      <c r="N32" s="39"/>
+      <c r="N32" s="40"/>
       <c r="O32" s="39"/>
       <c r="P32" s="39"/>
       <c r="Q32" s="39"/>
-      <c r="R32" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S32" s="51" t="s">
-        <v>80</v>
-      </c>
-      <c r="T32" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="U32" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="W32" s="4" t="s">
+      <c r="R32" s="39"/>
+      <c r="S32" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="T32" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="U32" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="V32" s="46" t="s">
         <v>80</v>
       </c>
       <c r="X32" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="33" spans="1:24">
+      <c r="Y32" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A33" s="5"/>
-      <c r="C33" s="69"/>
-      <c r="D33" s="69"/>
-      <c r="E33" s="69"/>
-      <c r="F33" s="69"/>
+      <c r="C33" s="82"/>
+      <c r="D33" s="82"/>
+      <c r="E33" s="82"/>
+      <c r="F33" s="82"/>
       <c r="G33" s="11" t="s">
         <v>69</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I33" s="78"/>
-      <c r="J33" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="K33" s="39"/>
-      <c r="L33" s="40"/>
+      <c r="I33" s="11">
+        <v>3</v>
+      </c>
+      <c r="J33" s="69"/>
+      <c r="K33" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="L33" s="39"/>
       <c r="M33" s="40"/>
-      <c r="N33" s="39"/>
+      <c r="N33" s="40"/>
       <c r="O33" s="39"/>
       <c r="P33" s="39"/>
       <c r="Q33" s="39"/>
-      <c r="R33" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S33" s="4" t="s">
+      <c r="R33" s="39"/>
+      <c r="S33" s="32" t="s">
         <v>80</v>
       </c>
       <c r="T33" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="U33" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="W33" s="43" t="s">
+      <c r="U33" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="V33" s="46" t="s">
+        <v>80</v>
+      </c>
+      <c r="X33" s="43" t="s">
         <v>139</v>
       </c>
-      <c r="X33" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="34" spans="1:24">
+      <c r="Y33" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A34" s="5"/>
-      <c r="C34" s="69"/>
-      <c r="D34" s="69"/>
-      <c r="E34" s="69"/>
-      <c r="F34" s="69"/>
+      <c r="C34" s="82"/>
+      <c r="D34" s="82"/>
+      <c r="E34" s="82"/>
+      <c r="F34" s="82"/>
       <c r="G34" s="11" t="s">
         <v>70</v>
       </c>
       <c r="H34" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="I34" s="78"/>
-      <c r="J34" s="18" t="s">
+      <c r="I34" s="11">
+        <v>4</v>
+      </c>
+      <c r="J34" s="69"/>
+      <c r="K34" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="K34" s="30" t="s">
-        <v>80</v>
-      </c>
       <c r="L34" s="30" t="s">
         <v>80</v>
       </c>
       <c r="M34" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="N34" s="53"/>
-      <c r="O34" s="53" t="s">
-        <v>80</v>
-      </c>
+      <c r="N34" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="O34" s="53"/>
       <c r="P34" s="53" t="s">
         <v>80</v>
       </c>
       <c r="Q34" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="R34" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S34" s="54" t="s">
+      <c r="R34" s="53" t="s">
+        <v>80</v>
+      </c>
+      <c r="S34" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="T34" s="54" t="s">
         <v>121</v>
       </c>
-      <c r="T34" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="U34" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="W34" s="64" t="s">
+      <c r="U34" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="V34" s="46" t="s">
+        <v>80</v>
+      </c>
+      <c r="X34" s="64" t="s">
         <v>139</v>
       </c>
-      <c r="X34" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="35" spans="1:24">
+      <c r="Y34" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A35" s="5"/>
-      <c r="C35" s="69"/>
-      <c r="D35" s="69"/>
-      <c r="E35" s="69"/>
-      <c r="F35" s="69"/>
+      <c r="C35" s="82"/>
+      <c r="D35" s="82"/>
+      <c r="E35" s="82"/>
+      <c r="F35" s="82"/>
       <c r="G35" s="11" t="s">
         <v>70</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="I35" s="78"/>
-      <c r="J35" s="18" t="s">
+      <c r="I35" s="11">
+        <v>5</v>
+      </c>
+      <c r="J35" s="69"/>
+      <c r="K35" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="K35" s="30" t="s">
-        <v>80</v>
-      </c>
       <c r="L35" s="30" t="s">
         <v>80</v>
       </c>
       <c r="M35" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="N35" s="53"/>
-      <c r="O35" s="53" t="s">
-        <v>80</v>
-      </c>
+      <c r="N35" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="O35" s="53"/>
       <c r="P35" s="53" t="s">
         <v>80</v>
       </c>
       <c r="Q35" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="R35" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S35" s="54" t="s">
+      <c r="R35" s="53" t="s">
+        <v>80</v>
+      </c>
+      <c r="S35" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="T35" s="54" t="s">
         <v>122</v>
       </c>
-      <c r="T35" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="U35" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="W35" s="43" t="s">
+      <c r="U35" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="V35" s="46" t="s">
+        <v>80</v>
+      </c>
+      <c r="X35" s="43" t="s">
         <v>139</v>
       </c>
-      <c r="X35" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="36" spans="1:24" s="2" customFormat="1" ht="16" thickBot="1">
+      <c r="Y35" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" s="2" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10"/>
       <c r="B36" s="7"/>
-      <c r="C36" s="70"/>
-      <c r="D36" s="70"/>
-      <c r="E36" s="70"/>
-      <c r="F36" s="70"/>
+      <c r="C36" s="83"/>
+      <c r="D36" s="83"/>
+      <c r="E36" s="83"/>
+      <c r="F36" s="83"/>
       <c r="G36" s="10" t="s">
         <v>70</v>
       </c>
       <c r="H36" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="I36" s="79"/>
-      <c r="J36" s="17" t="s">
+      <c r="I36" s="10">
+        <v>6</v>
+      </c>
+      <c r="J36" s="70"/>
+      <c r="K36" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="K36" s="44" t="s">
-        <v>80</v>
-      </c>
-      <c r="L36" s="65" t="s">
-        <v>80</v>
-      </c>
-      <c r="M36" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="N36" s="36"/>
-      <c r="O36" s="36" t="s">
-        <v>80</v>
-      </c>
+      <c r="L36" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="M36" s="65" t="s">
+        <v>80</v>
+      </c>
+      <c r="N36" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="O36" s="36"/>
       <c r="P36" s="36" t="s">
         <v>80</v>
       </c>
       <c r="Q36" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="R36" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="S36" s="17" t="s">
+      <c r="R36" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="S36" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="T36" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="T36" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="U36" s="17" t="s">
+      <c r="U36" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="V36" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="V36" s="36"/>
-      <c r="W36" s="55" t="s">
+      <c r="W36" s="36"/>
+      <c r="X36" s="55" t="s">
         <v>139</v>
       </c>
-      <c r="X36" s="36" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="37" spans="1:24">
+      <c r="Y36" s="36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B37" s="1">
         <v>42983</v>
       </c>
-      <c r="C37" s="68">
+      <c r="C37" s="81">
         <v>18.5</v>
       </c>
-      <c r="D37" s="68">
+      <c r="D37" s="81">
         <v>82</v>
       </c>
-      <c r="E37" s="68">
+      <c r="E37" s="81">
         <v>0.64</v>
       </c>
-      <c r="F37" s="68">
+      <c r="F37" s="81">
         <v>0.69</v>
       </c>
       <c r="G37" s="5" t="s">
@@ -3037,301 +3159,319 @@
       <c r="H37" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="I37" s="77"/>
-      <c r="J37" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="K37" s="37"/>
-      <c r="L37" s="38"/>
+      <c r="I37" s="11">
+        <v>1</v>
+      </c>
+      <c r="J37" s="68"/>
+      <c r="K37" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="L37" s="37"/>
       <c r="M37" s="38"/>
-      <c r="N37" s="37"/>
+      <c r="N37" s="38"/>
       <c r="O37" s="37"/>
       <c r="P37" s="37"/>
       <c r="Q37" s="37"/>
-      <c r="R37" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S37" s="4" t="s">
+      <c r="R37" s="37"/>
+      <c r="S37" s="32" t="s">
         <v>80</v>
       </c>
       <c r="T37" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="U37" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="W37" s="64" t="s">
+      <c r="U37" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="V37" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="X37" s="64" t="s">
         <v>142</v>
       </c>
-      <c r="X37" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" spans="1:24">
+      <c r="Y37" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A38" s="5"/>
-      <c r="C38" s="69"/>
-      <c r="D38" s="69"/>
-      <c r="E38" s="69"/>
-      <c r="F38" s="69"/>
+      <c r="C38" s="82"/>
+      <c r="D38" s="82"/>
+      <c r="E38" s="82"/>
+      <c r="F38" s="82"/>
       <c r="G38" s="11" t="s">
         <v>69</v>
       </c>
       <c r="H38" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="I38" s="78"/>
-      <c r="J38" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="K38" s="39"/>
-      <c r="L38" s="40"/>
+      <c r="I38" s="11">
+        <v>2</v>
+      </c>
+      <c r="J38" s="69"/>
+      <c r="K38" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="L38" s="39"/>
       <c r="M38" s="40"/>
-      <c r="N38" s="39"/>
+      <c r="N38" s="40"/>
       <c r="O38" s="39"/>
       <c r="P38" s="39"/>
       <c r="Q38" s="39"/>
-      <c r="R38" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S38" s="4" t="s">
+      <c r="R38" s="39"/>
+      <c r="S38" s="32" t="s">
         <v>80</v>
       </c>
       <c r="T38" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="U38" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="W38" s="4" t="s">
+      <c r="U38" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="V38" s="30" t="s">
         <v>80</v>
       </c>
       <c r="X38" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="39" spans="1:24">
+      <c r="Y38" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A39" s="5"/>
-      <c r="C39" s="69"/>
-      <c r="D39" s="69"/>
-      <c r="E39" s="69"/>
-      <c r="F39" s="69"/>
+      <c r="C39" s="82"/>
+      <c r="D39" s="82"/>
+      <c r="E39" s="82"/>
+      <c r="F39" s="82"/>
       <c r="G39" s="11" t="s">
         <v>69</v>
       </c>
       <c r="H39" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="I39" s="78"/>
-      <c r="J39" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="K39" s="39"/>
-      <c r="L39" s="40"/>
+      <c r="I39" s="11">
+        <v>3</v>
+      </c>
+      <c r="J39" s="69"/>
+      <c r="K39" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="L39" s="39"/>
       <c r="M39" s="40"/>
-      <c r="N39" s="39"/>
+      <c r="N39" s="40"/>
       <c r="O39" s="39"/>
       <c r="P39" s="39"/>
       <c r="Q39" s="39"/>
-      <c r="R39" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S39" s="4" t="s">
+      <c r="R39" s="39"/>
+      <c r="S39" s="32" t="s">
         <v>80</v>
       </c>
       <c r="T39" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="U39" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="W39" s="4" t="s">
+      <c r="U39" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="V39" s="30" t="s">
         <v>80</v>
       </c>
       <c r="X39" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="40" spans="1:24">
+      <c r="Y39" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A40" s="5"/>
-      <c r="C40" s="69"/>
-      <c r="D40" s="69"/>
-      <c r="E40" s="69"/>
-      <c r="F40" s="69"/>
+      <c r="C40" s="82"/>
+      <c r="D40" s="82"/>
+      <c r="E40" s="82"/>
+      <c r="F40" s="82"/>
       <c r="G40" s="11" t="s">
         <v>70</v>
       </c>
       <c r="H40" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="I40" s="78"/>
-      <c r="J40" s="18" t="s">
+      <c r="I40" s="11">
+        <v>4</v>
+      </c>
+      <c r="J40" s="69"/>
+      <c r="K40" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="K40" s="45" t="s">
-        <v>80</v>
-      </c>
-      <c r="L40" s="66" t="s">
-        <v>80</v>
-      </c>
-      <c r="M40" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="N40" s="53"/>
-      <c r="O40" s="53" t="s">
-        <v>80</v>
-      </c>
+      <c r="L40" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="M40" s="66" t="s">
+        <v>80</v>
+      </c>
+      <c r="N40" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="O40" s="53"/>
       <c r="P40" s="53" t="s">
         <v>80</v>
       </c>
       <c r="Q40" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="R40" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S40" s="54" t="s">
+      <c r="R40" s="53" t="s">
+        <v>80</v>
+      </c>
+      <c r="S40" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="T40" s="54" t="s">
         <v>85</v>
       </c>
-      <c r="T40" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="U40" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="W40" s="64" t="s">
+      <c r="U40" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="V40" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="X40" s="64" t="s">
         <v>143</v>
       </c>
-      <c r="X40" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="41" spans="1:24">
+      <c r="Y40" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A41" s="5"/>
-      <c r="C41" s="69"/>
-      <c r="D41" s="69"/>
-      <c r="E41" s="69"/>
-      <c r="F41" s="69"/>
+      <c r="C41" s="82"/>
+      <c r="D41" s="82"/>
+      <c r="E41" s="82"/>
+      <c r="F41" s="82"/>
       <c r="G41" s="11" t="s">
         <v>70</v>
       </c>
       <c r="H41" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="I41" s="78"/>
-      <c r="J41" s="18" t="s">
+      <c r="I41" s="11">
+        <v>5</v>
+      </c>
+      <c r="J41" s="69"/>
+      <c r="K41" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="K41" s="30" t="s">
-        <v>80</v>
-      </c>
       <c r="L41" s="30" t="s">
         <v>80</v>
       </c>
       <c r="M41" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="N41" s="53"/>
-      <c r="O41" s="59" t="s">
+      <c r="N41" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="O41" s="53"/>
+      <c r="P41" s="59" t="s">
         <v>139</v>
       </c>
-      <c r="P41" s="53" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q41" s="51" t="s">
-        <v>80</v>
-      </c>
-      <c r="R41" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S41" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="T41" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="U41" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="W41" s="43" t="s">
+      <c r="Q41" s="53" t="s">
+        <v>80</v>
+      </c>
+      <c r="R41" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="S41" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="T41" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="U41" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="V41" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="X41" s="43" t="s">
         <v>139</v>
       </c>
-      <c r="X41" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="42" spans="1:24" s="2" customFormat="1" ht="16" thickBot="1">
+      <c r="Y41" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" s="2" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
       <c r="B42" s="7"/>
-      <c r="C42" s="70"/>
-      <c r="D42" s="70"/>
-      <c r="E42" s="70"/>
-      <c r="F42" s="70"/>
+      <c r="C42" s="83"/>
+      <c r="D42" s="83"/>
+      <c r="E42" s="83"/>
+      <c r="F42" s="83"/>
       <c r="G42" s="10" t="s">
         <v>70</v>
       </c>
       <c r="H42" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="I42" s="79"/>
-      <c r="J42" s="17" t="s">
+      <c r="I42" s="10">
+        <v>6</v>
+      </c>
+      <c r="J42" s="70"/>
+      <c r="K42" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="K42" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="L42" s="31" t="s">
+      <c r="L42" s="36" t="s">
         <v>80</v>
       </c>
       <c r="M42" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="N42" s="36"/>
-      <c r="O42" s="55" t="s">
+      <c r="N42" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="O42" s="36"/>
+      <c r="P42" s="55" t="s">
         <v>139</v>
       </c>
-      <c r="P42" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q42" s="44" t="s">
-        <v>80</v>
-      </c>
-      <c r="R42" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="S42" s="36" t="s">
+      <c r="Q42" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="R42" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="S42" s="31" t="s">
         <v>80</v>
       </c>
       <c r="T42" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="U42" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="V42" s="36"/>
-      <c r="W42" s="63" t="s">
+      <c r="U42" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="V42" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="W42" s="36"/>
+      <c r="X42" s="63" t="s">
         <v>141</v>
       </c>
-      <c r="X42" s="36" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="43" spans="1:24">
+      <c r="Y42" s="36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B43" s="1">
         <v>42985</v>
       </c>
-      <c r="C43" s="68">
+      <c r="C43" s="81">
         <v>13</v>
       </c>
-      <c r="D43" s="68">
+      <c r="D43" s="81">
         <v>53</v>
       </c>
-      <c r="E43" s="68">
+      <c r="E43" s="81">
         <v>0.64</v>
       </c>
-      <c r="F43" s="68">
+      <c r="F43" s="81">
         <v>0.68</v>
       </c>
       <c r="G43" s="5" t="s">
@@ -3340,301 +3480,319 @@
       <c r="H43" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="I43" s="77"/>
-      <c r="J43" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="K43" s="37"/>
-      <c r="L43" s="38"/>
+      <c r="I43" s="11">
+        <v>1</v>
+      </c>
+      <c r="J43" s="68"/>
+      <c r="K43" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="L43" s="37"/>
       <c r="M43" s="38"/>
-      <c r="N43" s="39"/>
+      <c r="N43" s="38"/>
       <c r="O43" s="39"/>
       <c r="P43" s="39"/>
       <c r="Q43" s="39"/>
-      <c r="R43" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S43" s="51" t="s">
-        <v>80</v>
-      </c>
-      <c r="T43" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="U43" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="W43" s="61" t="s">
+      <c r="R43" s="39"/>
+      <c r="S43" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="T43" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="U43" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="V43" s="46" t="s">
+        <v>80</v>
+      </c>
+      <c r="X43" s="61" t="s">
         <v>141</v>
       </c>
-      <c r="X43" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="44" spans="1:24">
+      <c r="Y43" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A44" s="5"/>
-      <c r="C44" s="69"/>
-      <c r="D44" s="69"/>
-      <c r="E44" s="69"/>
-      <c r="F44" s="69"/>
+      <c r="C44" s="82"/>
+      <c r="D44" s="82"/>
+      <c r="E44" s="82"/>
+      <c r="F44" s="82"/>
       <c r="G44" s="11" t="s">
         <v>69</v>
       </c>
       <c r="H44" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="I44" s="78"/>
-      <c r="J44" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="K44" s="39"/>
-      <c r="L44" s="40"/>
+      <c r="I44" s="11">
+        <v>2</v>
+      </c>
+      <c r="J44" s="69"/>
+      <c r="K44" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="L44" s="39"/>
       <c r="M44" s="40"/>
-      <c r="N44" s="39"/>
+      <c r="N44" s="40"/>
       <c r="O44" s="39"/>
       <c r="P44" s="39"/>
       <c r="Q44" s="39"/>
-      <c r="R44" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S44" s="51" t="s">
-        <v>80</v>
-      </c>
-      <c r="T44" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="U44" s="18" t="s">
+      <c r="R44" s="39"/>
+      <c r="S44" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="T44" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="U44" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="V44" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="W44" s="64" t="s">
+      <c r="X44" s="64" t="s">
         <v>141</v>
       </c>
-      <c r="X44" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="45" spans="1:24">
+      <c r="Y44" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A45" s="5"/>
-      <c r="C45" s="69"/>
-      <c r="D45" s="69"/>
-      <c r="E45" s="69"/>
-      <c r="F45" s="69"/>
+      <c r="C45" s="82"/>
+      <c r="D45" s="82"/>
+      <c r="E45" s="82"/>
+      <c r="F45" s="82"/>
       <c r="G45" s="11" t="s">
         <v>69</v>
       </c>
       <c r="H45" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="I45" s="78"/>
-      <c r="J45" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="K45" s="39"/>
-      <c r="L45" s="40"/>
+      <c r="I45" s="11">
+        <v>3</v>
+      </c>
+      <c r="J45" s="69"/>
+      <c r="K45" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="L45" s="39"/>
       <c r="M45" s="40"/>
-      <c r="N45" s="39"/>
+      <c r="N45" s="40"/>
       <c r="O45" s="39"/>
       <c r="P45" s="39"/>
       <c r="Q45" s="39"/>
-      <c r="R45" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S45" s="51" t="s">
-        <v>80</v>
-      </c>
-      <c r="T45" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="U45" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="W45" s="4" t="s">
+      <c r="R45" s="39"/>
+      <c r="S45" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="T45" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="U45" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="V45" s="46" t="s">
         <v>80</v>
       </c>
       <c r="X45" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="46" spans="1:24">
+      <c r="Y45" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A46" s="5"/>
-      <c r="C46" s="69"/>
-      <c r="D46" s="69"/>
-      <c r="E46" s="69"/>
-      <c r="F46" s="69"/>
+      <c r="C46" s="82"/>
+      <c r="D46" s="82"/>
+      <c r="E46" s="82"/>
+      <c r="F46" s="82"/>
       <c r="G46" s="11" t="s">
         <v>70</v>
       </c>
       <c r="H46" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="I46" s="78"/>
-      <c r="J46" s="18" t="s">
+      <c r="I46" s="11">
+        <v>4</v>
+      </c>
+      <c r="J46" s="69"/>
+      <c r="K46" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="K46" s="30" t="s">
-        <v>80</v>
-      </c>
       <c r="L46" s="30" t="s">
         <v>80</v>
       </c>
       <c r="M46" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="N46" s="53"/>
-      <c r="O46" s="53" t="s">
-        <v>80</v>
-      </c>
+      <c r="N46" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="O46" s="53"/>
       <c r="P46" s="53" t="s">
         <v>80</v>
       </c>
       <c r="Q46" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="R46" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S46" s="54" t="s">
+      <c r="R46" s="53" t="s">
+        <v>80</v>
+      </c>
+      <c r="S46" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="T46" s="54" t="s">
         <v>87</v>
       </c>
-      <c r="T46" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="U46" s="54" t="s">
+      <c r="U46" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="V46" s="54" t="s">
         <v>124</v>
       </c>
-      <c r="W46" s="43" t="s">
+      <c r="X46" s="43" t="s">
         <v>139</v>
       </c>
-      <c r="X46" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="47" spans="1:24">
+      <c r="Y46" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A47" s="5"/>
-      <c r="C47" s="69"/>
-      <c r="D47" s="69"/>
-      <c r="E47" s="69"/>
-      <c r="F47" s="69"/>
+      <c r="C47" s="82"/>
+      <c r="D47" s="82"/>
+      <c r="E47" s="82"/>
+      <c r="F47" s="82"/>
       <c r="G47" s="11" t="s">
         <v>70</v>
       </c>
       <c r="H47" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="I47" s="78"/>
-      <c r="J47" s="18" t="s">
+      <c r="I47" s="11">
+        <v>5</v>
+      </c>
+      <c r="J47" s="69"/>
+      <c r="K47" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="K47" s="30" t="s">
-        <v>80</v>
-      </c>
       <c r="L47" s="30" t="s">
         <v>80</v>
       </c>
       <c r="M47" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="N47" s="53"/>
-      <c r="O47" s="53" t="s">
-        <v>80</v>
-      </c>
+      <c r="N47" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="O47" s="53"/>
       <c r="P47" s="53" t="s">
         <v>80</v>
       </c>
       <c r="Q47" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="R47" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S47" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="T47" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="U47" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="W47" s="64" t="s">
+      <c r="R47" s="53" t="s">
+        <v>80</v>
+      </c>
+      <c r="S47" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="T47" s="46" t="s">
+        <v>80</v>
+      </c>
+      <c r="U47" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="V47" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="X47" s="64" t="s">
         <v>139</v>
       </c>
-      <c r="X47" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="48" spans="1:24" s="2" customFormat="1" ht="16" thickBot="1">
+      <c r="Y47" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25" s="2" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
       <c r="B48" s="7"/>
-      <c r="C48" s="70"/>
-      <c r="D48" s="70"/>
-      <c r="E48" s="70"/>
-      <c r="F48" s="70"/>
+      <c r="C48" s="83"/>
+      <c r="D48" s="83"/>
+      <c r="E48" s="83"/>
+      <c r="F48" s="83"/>
       <c r="G48" s="10" t="s">
         <v>70</v>
       </c>
       <c r="H48" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="I48" s="79"/>
-      <c r="J48" s="17" t="s">
+      <c r="I48" s="10">
+        <v>6</v>
+      </c>
+      <c r="J48" s="70"/>
+      <c r="K48" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="K48" s="36" t="s">
-        <v>80</v>
-      </c>
       <c r="L48" s="36" t="s">
         <v>80</v>
       </c>
       <c r="M48" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="N48" s="36"/>
-      <c r="O48" s="36" t="s">
-        <v>80</v>
-      </c>
+      <c r="N48" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="O48" s="36"/>
       <c r="P48" s="36" t="s">
         <v>80</v>
       </c>
       <c r="Q48" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="R48" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="S48" s="36" t="s">
+      <c r="R48" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="S48" s="31" t="s">
         <v>80</v>
       </c>
       <c r="T48" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="U48" s="55" t="s">
+      <c r="U48" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="V48" s="55" t="s">
         <v>125</v>
       </c>
-      <c r="V48" s="36"/>
-      <c r="W48" s="55" t="s">
+      <c r="W48" s="36"/>
+      <c r="X48" s="55" t="s">
         <v>139</v>
       </c>
-      <c r="X48" s="36" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="49" spans="1:24">
+      <c r="Y48" s="36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="49" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
         <v>48</v>
       </c>
       <c r="B49" s="1">
         <v>42992</v>
       </c>
-      <c r="C49" s="68">
+      <c r="C49" s="81">
         <v>16.5</v>
       </c>
-      <c r="D49" s="68">
+      <c r="D49" s="81">
         <v>48</v>
       </c>
-      <c r="E49" s="68">
+      <c r="E49" s="81">
         <v>0.96</v>
       </c>
-      <c r="F49" s="68">
+      <c r="F49" s="81">
         <v>0.99</v>
       </c>
       <c r="G49" s="5" t="s">
@@ -3643,33 +3801,33 @@
       <c r="H49" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="I49" s="77"/>
-      <c r="J49" s="18" t="s">
+      <c r="I49" s="11">
+        <v>1</v>
+      </c>
+      <c r="J49" s="68"/>
+      <c r="K49" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="K49" s="46" t="s">
-        <v>80</v>
-      </c>
       <c r="L49" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="M49" s="18" t="s">
+      <c r="M49" s="46" t="s">
+        <v>80</v>
+      </c>
+      <c r="N49" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="N49" s="52"/>
-      <c r="O49" s="58" t="s">
+      <c r="O49" s="52"/>
+      <c r="P49" s="58" t="s">
         <v>139</v>
       </c>
-      <c r="P49" s="52" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q49" s="62" t="s">
-        <v>80</v>
-      </c>
-      <c r="R49" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S49" s="4" t="s">
+      <c r="Q49" s="52" t="s">
+        <v>80</v>
+      </c>
+      <c r="R49" s="62" t="s">
+        <v>80</v>
+      </c>
+      <c r="S49" s="32" t="s">
         <v>80</v>
       </c>
       <c r="T49" s="4" t="s">
@@ -3678,40 +3836,43 @@
       <c r="U49" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="W49" s="4" t="s">
+      <c r="V49" s="4" t="s">
         <v>80</v>
       </c>
       <c r="X49" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="50" spans="1:24">
+      <c r="Y49" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A50" s="5"/>
-      <c r="C50" s="69"/>
-      <c r="D50" s="69"/>
-      <c r="E50" s="69"/>
-      <c r="F50" s="69"/>
+      <c r="C50" s="82"/>
+      <c r="D50" s="82"/>
+      <c r="E50" s="82"/>
+      <c r="F50" s="82"/>
       <c r="G50" s="11" t="s">
         <v>69</v>
       </c>
       <c r="H50" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="I50" s="80"/>
-      <c r="J50" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="K50" s="39"/>
+      <c r="I50" s="11">
+        <v>2</v>
+      </c>
+      <c r="J50" s="80"/>
+      <c r="K50" s="32" t="s">
+        <v>80</v>
+      </c>
       <c r="L50" s="39"/>
       <c r="M50" s="39"/>
       <c r="N50" s="39"/>
       <c r="O50" s="39"/>
       <c r="P50" s="39"/>
       <c r="Q50" s="39"/>
-      <c r="R50" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S50" s="4" t="s">
+      <c r="R50" s="39"/>
+      <c r="S50" s="32" t="s">
         <v>80</v>
       </c>
       <c r="T50" s="4" t="s">
@@ -3720,274 +3881,274 @@
       <c r="U50" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="W50" s="43" t="s">
+      <c r="V50" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="X50" s="43" t="s">
         <v>139</v>
       </c>
-      <c r="X50" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="51" spans="1:24">
+      <c r="Y50" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="51" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A51" s="5"/>
-      <c r="C51" s="69"/>
-      <c r="D51" s="69"/>
-      <c r="E51" s="69"/>
-      <c r="F51" s="69"/>
+      <c r="C51" s="82"/>
+      <c r="D51" s="82"/>
+      <c r="E51" s="82"/>
+      <c r="F51" s="82"/>
       <c r="G51" s="11" t="s">
         <v>69</v>
       </c>
       <c r="H51" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="I51" s="80"/>
-      <c r="J51" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="K51" s="39"/>
+      <c r="I51" s="11">
+        <v>3</v>
+      </c>
+      <c r="J51" s="80"/>
+      <c r="K51" s="32" t="s">
+        <v>80</v>
+      </c>
       <c r="L51" s="39"/>
       <c r="M51" s="39"/>
       <c r="N51" s="39"/>
       <c r="O51" s="39"/>
       <c r="P51" s="39"/>
       <c r="Q51" s="39"/>
-      <c r="R51" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S51" s="4" t="s">
+      <c r="R51" s="39"/>
+      <c r="S51" s="32" t="s">
         <v>80</v>
       </c>
       <c r="T51" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="U51" s="43" t="s">
+      <c r="U51" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="V51" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="W51" s="4" t="s">
-        <v>80</v>
-      </c>
       <c r="X51" s="4" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="52" spans="1:24">
+      <c r="Y51" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="52" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A52" s="5"/>
-      <c r="C52" s="69"/>
-      <c r="D52" s="69"/>
-      <c r="E52" s="69"/>
-      <c r="F52" s="69"/>
+      <c r="C52" s="82"/>
+      <c r="D52" s="82"/>
+      <c r="E52" s="82"/>
+      <c r="F52" s="82"/>
       <c r="G52" s="11" t="s">
         <v>70</v>
       </c>
       <c r="H52" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="I52" s="80"/>
-      <c r="J52" s="18" t="s">
+      <c r="I52" s="11">
+        <v>4</v>
+      </c>
+      <c r="J52" s="80"/>
+      <c r="K52" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="K52" s="46" t="s">
-        <v>80</v>
-      </c>
       <c r="L52" s="46" t="s">
         <v>80</v>
       </c>
       <c r="M52" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="N52" s="53"/>
-      <c r="O52" s="53" t="s">
-        <v>80</v>
-      </c>
+      <c r="N52" s="46" t="s">
+        <v>80</v>
+      </c>
+      <c r="O52" s="53"/>
       <c r="P52" s="53" t="s">
         <v>80</v>
       </c>
       <c r="Q52" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="R52" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S52" s="56" t="s">
+      <c r="R52" s="53" t="s">
+        <v>80</v>
+      </c>
+      <c r="S52" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="T52" s="56" t="s">
         <v>137</v>
       </c>
-      <c r="T52" s="4" t="s">
-        <v>80</v>
-      </c>
       <c r="U52" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="W52" s="43" t="s">
+      <c r="V52" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="X52" s="43" t="s">
         <v>139</v>
       </c>
-      <c r="X52" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="53" spans="1:24">
+      <c r="Y52" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A53" s="5"/>
-      <c r="C53" s="69"/>
-      <c r="D53" s="69"/>
-      <c r="E53" s="69"/>
-      <c r="F53" s="69"/>
+      <c r="C53" s="82"/>
+      <c r="D53" s="82"/>
+      <c r="E53" s="82"/>
+      <c r="F53" s="82"/>
       <c r="G53" s="11" t="s">
         <v>70</v>
       </c>
       <c r="H53" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="I53" s="80"/>
-      <c r="J53" s="18" t="s">
+      <c r="I53" s="11">
+        <v>5</v>
+      </c>
+      <c r="J53" s="80"/>
+      <c r="K53" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="K53" s="46" t="s">
-        <v>80</v>
-      </c>
       <c r="L53" s="46" t="s">
         <v>80</v>
       </c>
       <c r="M53" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="N53" s="53"/>
-      <c r="O53" s="53" t="s">
-        <v>80</v>
-      </c>
+      <c r="N53" s="46" t="s">
+        <v>80</v>
+      </c>
+      <c r="O53" s="53"/>
       <c r="P53" s="53" t="s">
         <v>80</v>
       </c>
       <c r="Q53" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="R53" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="S53" s="56" t="s">
+      <c r="R53" s="53" t="s">
+        <v>80</v>
+      </c>
+      <c r="S53" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="T53" s="56" t="s">
         <v>136</v>
       </c>
-      <c r="T53" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="U53" s="43" t="s">
+      <c r="U53" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="V53" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="W53" s="43" t="s">
+      <c r="X53" s="43" t="s">
         <v>139</v>
       </c>
-      <c r="X53" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="54" spans="1:24" s="2" customFormat="1" ht="16" thickBot="1">
+      <c r="Y53" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="54" spans="1:25" s="2" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="10"/>
       <c r="B54" s="7"/>
-      <c r="C54" s="70"/>
-      <c r="D54" s="70"/>
-      <c r="E54" s="70"/>
-      <c r="F54" s="70"/>
+      <c r="C54" s="83"/>
+      <c r="D54" s="83"/>
+      <c r="E54" s="83"/>
+      <c r="F54" s="83"/>
       <c r="G54" s="10" t="s">
         <v>70</v>
       </c>
       <c r="H54" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="I54" s="79"/>
-      <c r="J54" s="17" t="s">
+      <c r="I54" s="12">
+        <v>6</v>
+      </c>
+      <c r="J54" s="70"/>
+      <c r="K54" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="K54" s="36" t="s">
-        <v>80</v>
-      </c>
       <c r="L54" s="36" t="s">
         <v>80</v>
       </c>
       <c r="M54" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="N54" s="36"/>
-      <c r="O54" s="36" t="s">
-        <v>80</v>
-      </c>
+      <c r="N54" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="O54" s="36"/>
       <c r="P54" s="36" t="s">
         <v>80</v>
       </c>
       <c r="Q54" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="R54" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="S54" s="57" t="s">
+      <c r="R54" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="S54" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="T54" s="57" t="s">
         <v>135</v>
       </c>
-      <c r="T54" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="U54" s="55" t="s">
+      <c r="U54" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="V54" s="55" t="s">
         <v>82</v>
       </c>
-      <c r="V54" s="36"/>
-      <c r="W54" s="55" t="s">
+      <c r="W54" s="36"/>
+      <c r="X54" s="55" t="s">
         <v>139</v>
       </c>
-      <c r="X54" s="36" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="55" spans="1:24" ht="16" thickBot="1"/>
-    <row r="56" spans="1:24">
+      <c r="Y54" s="36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="55" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C56" s="33"/>
       <c r="D56" s="33"/>
       <c r="E56" s="33"/>
       <c r="F56" s="33"/>
       <c r="G56" s="33"/>
-      <c r="S56" s="71" t="s">
+      <c r="T56" s="74" t="s">
         <v>88</v>
       </c>
-      <c r="T56" s="72"/>
-    </row>
-    <row r="57" spans="1:24">
-      <c r="S57" s="73"/>
-      <c r="T57" s="74"/>
-    </row>
-    <row r="58" spans="1:24" ht="45" customHeight="1">
+      <c r="U56" s="75"/>
+    </row>
+    <row r="57" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="T57" s="76"/>
+      <c r="U57" s="77"/>
+    </row>
+    <row r="58" spans="1:25" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C58" s="33"/>
       <c r="D58" s="33"/>
       <c r="E58" s="33"/>
       <c r="F58" s="33"/>
-      <c r="S58" s="73" t="s">
+      <c r="T58" s="76" t="s">
         <v>89</v>
       </c>
-      <c r="T58" s="74"/>
-    </row>
-    <row r="59" spans="1:24" ht="16" thickBot="1">
-      <c r="S59" s="75"/>
-      <c r="T59" s="76"/>
+      <c r="U58" s="77"/>
+    </row>
+    <row r="59" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="T59" s="78"/>
+      <c r="U59" s="79"/>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="I31:I36"/>
-    <mergeCell ref="I2:I6"/>
-    <mergeCell ref="I7:I12"/>
-    <mergeCell ref="I13:I18"/>
-    <mergeCell ref="I19:I24"/>
-    <mergeCell ref="I25:I30"/>
-    <mergeCell ref="S56:T57"/>
-    <mergeCell ref="S58:T59"/>
-    <mergeCell ref="I37:I42"/>
-    <mergeCell ref="I43:I48"/>
-    <mergeCell ref="I49:I54"/>
-    <mergeCell ref="C49:C54"/>
-    <mergeCell ref="D49:D54"/>
-    <mergeCell ref="E49:E54"/>
-    <mergeCell ref="F49:F54"/>
-    <mergeCell ref="C37:C42"/>
-    <mergeCell ref="D37:D42"/>
-    <mergeCell ref="E37:E42"/>
-    <mergeCell ref="F37:F42"/>
-    <mergeCell ref="C43:C48"/>
-    <mergeCell ref="D43:D48"/>
-    <mergeCell ref="E43:E48"/>
-    <mergeCell ref="F43:F48"/>
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="D2:D6"/>
+    <mergeCell ref="E2:E6"/>
+    <mergeCell ref="F2:F6"/>
+    <mergeCell ref="C7:C12"/>
+    <mergeCell ref="D7:D12"/>
+    <mergeCell ref="E7:E12"/>
+    <mergeCell ref="F7:F12"/>
     <mergeCell ref="C31:C36"/>
     <mergeCell ref="D31:D36"/>
     <mergeCell ref="E31:E36"/>
@@ -4004,14 +4165,29 @@
     <mergeCell ref="D19:D24"/>
     <mergeCell ref="E19:E24"/>
     <mergeCell ref="F19:F24"/>
-    <mergeCell ref="C2:C6"/>
-    <mergeCell ref="D2:D6"/>
-    <mergeCell ref="E2:E6"/>
-    <mergeCell ref="F2:F6"/>
-    <mergeCell ref="C7:C12"/>
-    <mergeCell ref="D7:D12"/>
-    <mergeCell ref="E7:E12"/>
-    <mergeCell ref="F7:F12"/>
+    <mergeCell ref="C49:C54"/>
+    <mergeCell ref="D49:D54"/>
+    <mergeCell ref="E49:E54"/>
+    <mergeCell ref="F49:F54"/>
+    <mergeCell ref="C37:C42"/>
+    <mergeCell ref="D37:D42"/>
+    <mergeCell ref="E37:E42"/>
+    <mergeCell ref="F37:F42"/>
+    <mergeCell ref="C43:C48"/>
+    <mergeCell ref="D43:D48"/>
+    <mergeCell ref="E43:E48"/>
+    <mergeCell ref="F43:F48"/>
+    <mergeCell ref="T56:U57"/>
+    <mergeCell ref="T58:U59"/>
+    <mergeCell ref="J37:J42"/>
+    <mergeCell ref="J43:J48"/>
+    <mergeCell ref="J49:J54"/>
+    <mergeCell ref="J31:J36"/>
+    <mergeCell ref="J2:J6"/>
+    <mergeCell ref="J7:J12"/>
+    <mergeCell ref="J13:J18"/>
+    <mergeCell ref="J19:J24"/>
+    <mergeCell ref="J25:J30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="61" orientation="landscape" r:id="rId1"/>
@@ -4026,7 +4202,7 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
@@ -4038,7 +4214,7 @@
     <col min="8" max="8" width="28.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16" thickBot="1">
+    <row r="1" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>90</v>
       </c>
@@ -4064,7 +4240,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="22"/>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -4074,7 +4250,7 @@
       <c r="G2" s="23"/>
       <c r="H2" s="28"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
         <v>98</v>
       </c>
@@ -4100,7 +4276,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
         <v>102</v>
       </c>
@@ -4126,7 +4302,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="22"/>
       <c r="B5" s="23"/>
       <c r="C5" s="23"/>
@@ -4138,7 +4314,7 @@
       <c r="G5" s="23"/>
       <c r="H5" s="28"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
         <v>106</v>
       </c>
@@ -4162,7 +4338,7 @@
       </c>
       <c r="H6" s="28"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
         <v>107</v>
       </c>
@@ -4186,7 +4362,7 @@
       </c>
       <c r="H7" s="28"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
         <v>109</v>
       </c>
@@ -4210,7 +4386,7 @@
       </c>
       <c r="H8" s="28"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="22" t="s">
         <v>110</v>
       </c>
@@ -4234,7 +4410,7 @@
       </c>
       <c r="H9" s="28"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="22" t="s">
         <v>113</v>
       </c>
@@ -4260,7 +4436,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="22" t="s">
         <v>116</v>
       </c>
@@ -4284,7 +4460,7 @@
       </c>
       <c r="H11" s="28"/>
     </row>
-    <row r="12" spans="1:8" ht="16" thickBot="1">
+    <row r="12" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>118</v>
       </c>
@@ -4302,7 +4478,7 @@
       <c r="G12" s="23"/>
       <c r="H12" s="28"/>
     </row>
-    <row r="13" spans="1:8" ht="16" thickBot="1">
+    <row r="13" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
         <v>119</v>
       </c>

</xml_diff>